<commit_message>
Added the option to use a retention time table in place of explicit compound assignments in the IRMS export.
</commit_message>
<xml_diff>
--- a/GCIRMS_Processor/GCIRMS Template.xlsx
+++ b/GCIRMS_Processor/GCIRMS Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A429BC-44ED-48BF-9702-97D3B82C0F83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13481491-5DA0-4335-86D4-CC3F8D643B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <sheet name="Samples" sheetId="1" r:id="rId3"/>
     <sheet name="Standards" sheetId="2" r:id="rId4"/>
     <sheet name="Headers" sheetId="4" r:id="rId5"/>
-    <sheet name="Derivatization" sheetId="8" r:id="rId6"/>
-    <sheet name="Initials" sheetId="9" r:id="rId7"/>
+    <sheet name="Retention Times" sheetId="10" r:id="rId6"/>
+    <sheet name="Derivatization" sheetId="8" r:id="rId7"/>
+    <sheet name="Initials" sheetId="9" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Standards!$A$1:$G$38</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="264">
   <si>
     <t>id1</t>
   </si>
@@ -343,19 +344,10 @@
     <t>Isotope ratio relative to reference gas</t>
   </si>
   <si>
-    <t>Peak number in sample (unclear on functionality for non-Isodat users)</t>
-  </si>
-  <si>
     <t>Peak area in Volt-seconds (Vs)</t>
   </si>
   <si>
-    <t>Raw isotope ratio</t>
-  </si>
-  <si>
     <t>Injection row number</t>
-  </si>
-  <si>
-    <t>Peak retention time</t>
   </si>
   <si>
     <t>variable</t>
@@ -724,9 +716,6 @@
     <t>Peak height of mass 2 (mV)</t>
   </si>
   <si>
-    <t>Compound name and class (separated by a space)</t>
-  </si>
-  <si>
     <t>Description of the column's purpose.</t>
   </si>
   <si>
@@ -1109,6 +1098,110 @@
       </rPr>
       <t>, only the first seven columns are imported. If you need additional metadata columns, these can be added but the 'range' of the sample_info object in the 'ingest_function' of the Shiny App must be changed, too.</t>
     </r>
+  </si>
+  <si>
+    <t>(Optional) Raw isotope ratio</t>
+  </si>
+  <si>
+    <t>(Optional) Peak number in sample; if there are duplicate component rows, only the row with the highest peak number is used. This is the only filter for multiple compound observations per injection; if this is left blank or your software exports peak numbers differently, you will have problems!</t>
+  </si>
+  <si>
+    <t>(Quasi-optional) Peak retention time; only used if the Component column is empty and, if so, queries the Retention Times sheet to assign compound names.</t>
+  </si>
+  <si>
+    <t>(Quasi-optional) Compound name and class (separated by a space); default method of compound identificaiton. If empty, then compound names are assigned by retention time and the Retention Times sheet.</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>Retention Times</t>
+  </si>
+  <si>
+    <t>(Optional) A peak retention time look-up table to assign compound names.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Important! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>Compound names are assigned in one of two ways: using the 'Component' column of the raw IRMS export or by matching a peak's retention time to the matching time in this sheet. If both are present, then the 'Component' assignment is preferred.</t>
+    </r>
+  </si>
+  <si>
+    <t>C24 FAME</t>
+  </si>
+  <si>
+    <t>C30 FAME</t>
+  </si>
+  <si>
+    <t>C17 Alkane</t>
+  </si>
+  <si>
+    <t>C19 Alkane</t>
+  </si>
+  <si>
+    <t>C21 Alkane</t>
+  </si>
+  <si>
+    <t>C23 Alkane</t>
+  </si>
+  <si>
+    <t>C25 Alkane</t>
+  </si>
+  <si>
+    <t>C22 FAME</t>
+  </si>
+  <si>
+    <t>C22:1 FAME</t>
+  </si>
+  <si>
+    <t>C26 FAME</t>
+  </si>
+  <si>
+    <t>C28 FAME</t>
+  </si>
+  <si>
+    <t>C32 FAME</t>
+  </si>
+  <si>
+    <t>C34 FAME</t>
+  </si>
+  <si>
+    <t>C36 FAME</t>
+  </si>
+  <si>
+    <t>Compound name and class separated by a space.</t>
+  </si>
+  <si>
+    <t>Retention time in seconds.</t>
+  </si>
+  <si>
+    <t>Retention time window to assign peak in seconds.</t>
+  </si>
+  <si>
+    <t>Ref 1</t>
+  </si>
+  <si>
+    <t>Ref 2</t>
+  </si>
+  <si>
+    <t>Ref 3</t>
+  </si>
+  <si>
+    <t>compound_option</t>
+  </si>
+  <si>
+    <t>Assigned by IRMS export in Component/comp column.</t>
+  </si>
+  <si>
+    <t>Choose which method to assign peak names.</t>
   </si>
 </sst>
 </file>
@@ -1327,7 +1420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1434,7 +1527,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1445,6 +1541,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1769,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52BD4A5-5C4B-4F65-B4E7-6F2D013F4981}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1785,83 +1887,95 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>173</v>
-      </c>
       <c r="C2" s="14" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>174</v>
-      </c>
       <c r="C3" s="30" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>218</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>219</v>
+      <c r="A6" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>215</v>
       </c>
     </row>
+    <row r="8" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1949,7 +2063,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="R1" s="4"/>
       <c r="S1" s="4" t="s">
@@ -1959,10 +2073,10 @@
         <v>33</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -2019,7 +2133,7 @@
         <v>69</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="U2" s="7" t="str">
         <f>INDEX(T6:T7,MATCH([1]Samples!E2,'[1]Sequence Table'!S6:S7,0))</f>
@@ -2083,7 +2197,7 @@
         <v>67</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>72</v>
@@ -2195,10 +2309,10 @@
         <v>40.35</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -2312,7 +2426,7 @@
         <v>12</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -2413,7 +2527,7 @@
         <v>58.75</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
@@ -2621,18 +2735,18 @@
         <v>58.75</v>
       </c>
       <c r="S13" s="10"/>
-      <c r="T13" s="38" t="s">
-        <v>138</v>
+      <c r="T13" s="40" t="s">
+        <v>135</v>
       </c>
       <c r="U13" s="11"/>
-      <c r="V13" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="W13" s="39"/>
-      <c r="X13" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y13" s="40"/>
+      <c r="V13" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="W13" s="45"/>
+      <c r="X13" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y13" s="46"/>
       <c r="Z13" s="12"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -2686,12 +2800,12 @@
         <v>40.35</v>
       </c>
       <c r="S14" s="10"/>
-      <c r="T14" s="38"/>
+      <c r="T14" s="40"/>
       <c r="U14" s="11"/>
-      <c r="V14" s="39"/>
-      <c r="W14" s="39"/>
-      <c r="X14" s="40"/>
-      <c r="Y14" s="40"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
+      <c r="X14" s="46"/>
+      <c r="Y14" s="46"/>
       <c r="Z14" s="12"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -2745,12 +2859,12 @@
         <v>40.35</v>
       </c>
       <c r="S15" s="10"/>
-      <c r="T15" s="38"/>
+      <c r="T15" s="40"/>
       <c r="U15" s="11"/>
-      <c r="V15" s="39"/>
-      <c r="W15" s="39"/>
-      <c r="X15" s="40"/>
-      <c r="Y15" s="40"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="45"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="46"/>
       <c r="Z15" s="12"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
@@ -2804,18 +2918,18 @@
         <v>40.35</v>
       </c>
       <c r="S16" s="10"/>
-      <c r="T16" s="38" t="s">
-        <v>132</v>
+      <c r="T16" s="40" t="s">
+        <v>129</v>
       </c>
       <c r="U16" s="11"/>
-      <c r="V16" s="37" t="s">
+      <c r="V16" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="W16" s="37"/>
-      <c r="X16" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y16" s="38"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y16" s="40"/>
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -2869,12 +2983,12 @@
         <v>40.35</v>
       </c>
       <c r="S17" s="10"/>
-      <c r="T17" s="38"/>
+      <c r="T17" s="40"/>
       <c r="U17" s="11"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="37"/>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="38"/>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="40"/>
+      <c r="Y17" s="40"/>
       <c r="Z17" s="12"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -2928,12 +3042,12 @@
         <v>40.35</v>
       </c>
       <c r="S18" s="10"/>
-      <c r="T18" s="38"/>
+      <c r="T18" s="40"/>
       <c r="U18" s="11"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="38"/>
-      <c r="Y18" s="38"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="40"/>
       <c r="Z18" s="12"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
@@ -2987,18 +3101,18 @@
         <v>40.35</v>
       </c>
       <c r="S19" s="10"/>
-      <c r="T19" s="38" t="s">
-        <v>133</v>
+      <c r="T19" s="40" t="s">
+        <v>130</v>
       </c>
       <c r="U19" s="11"/>
-      <c r="V19" s="37" t="s">
+      <c r="V19" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="W19" s="37"/>
-      <c r="X19" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y19" s="38"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y19" s="40"/>
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -3052,12 +3166,12 @@
         <v>40.35</v>
       </c>
       <c r="S20" s="10"/>
-      <c r="T20" s="38"/>
+      <c r="T20" s="40"/>
       <c r="U20" s="11"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="38"/>
-      <c r="Y20" s="38"/>
+      <c r="V20" s="41"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="40"/>
       <c r="Z20" s="12"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -3111,12 +3225,12 @@
         <v>40.35</v>
       </c>
       <c r="S21" s="10"/>
-      <c r="T21" s="38"/>
+      <c r="T21" s="40"/>
       <c r="U21" s="11"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="38"/>
-      <c r="Y21" s="38"/>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="40"/>
+      <c r="Y21" s="40"/>
       <c r="Z21" s="12"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
@@ -3169,18 +3283,18 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T22" s="38" t="s">
-        <v>141</v>
+      <c r="T22" s="40" t="s">
+        <v>138</v>
       </c>
       <c r="U22" s="10"/>
-      <c r="V22" s="37" t="s">
+      <c r="V22" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="W22" s="37"/>
-      <c r="X22" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y22" s="38"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y22" s="40"/>
       <c r="Z22" s="12"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -3233,12 +3347,12 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T23" s="38"/>
+      <c r="T23" s="40"/>
       <c r="U23" s="10"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="38"/>
-      <c r="Y23" s="38"/>
+      <c r="V23" s="41"/>
+      <c r="W23" s="41"/>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="40"/>
       <c r="Z23" s="12"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -3289,12 +3403,12 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="T24" s="38"/>
+      <c r="T24" s="40"/>
       <c r="U24" s="10"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="37"/>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="38"/>
+      <c r="V24" s="41"/>
+      <c r="W24" s="41"/>
+      <c r="X24" s="40"/>
+      <c r="Y24" s="40"/>
       <c r="Z24" s="12"/>
     </row>
     <row r="25" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3345,18 +3459,18 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="T25" s="41" t="s">
-        <v>135</v>
+      <c r="T25" s="42" t="s">
+        <v>132</v>
       </c>
       <c r="U25" s="10"/>
-      <c r="V25" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="W25" s="37"/>
-      <c r="X25" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y25" s="38"/>
+      <c r="V25" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="W25" s="41"/>
+      <c r="X25" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y25" s="40"/>
       <c r="Z25" s="12"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3407,12 +3521,12 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="T26" s="42"/>
+      <c r="T26" s="43"/>
       <c r="U26" s="10"/>
-      <c r="V26" s="37"/>
-      <c r="W26" s="37"/>
-      <c r="X26" s="38"/>
-      <c r="Y26" s="38"/>
+      <c r="V26" s="41"/>
+      <c r="W26" s="41"/>
+      <c r="X26" s="40"/>
+      <c r="Y26" s="40"/>
       <c r="Z26" s="12"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -3463,12 +3577,12 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="T27" s="42"/>
+      <c r="T27" s="43"/>
       <c r="U27" s="10"/>
-      <c r="V27" s="37"/>
-      <c r="W27" s="37"/>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="38"/>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="40"/>
+      <c r="Y27" s="40"/>
       <c r="Z27" s="12"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
@@ -3519,16 +3633,16 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="T28" s="42"/>
+      <c r="T28" s="43"/>
       <c r="U28" s="10"/>
-      <c r="V28" s="37" t="s">
+      <c r="V28" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="W28" s="37"/>
-      <c r="X28" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y28" s="38"/>
+      <c r="W28" s="41"/>
+      <c r="X28" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y28" s="40"/>
       <c r="Z28" s="12"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -3579,12 +3693,12 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="T29" s="42"/>
+      <c r="T29" s="43"/>
       <c r="U29" s="10"/>
-      <c r="V29" s="37"/>
-      <c r="W29" s="37"/>
-      <c r="X29" s="38"/>
-      <c r="Y29" s="38"/>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="40"/>
       <c r="Z29" s="12"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -3637,12 +3751,12 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T30" s="43"/>
+      <c r="T30" s="44"/>
       <c r="U30" s="10"/>
-      <c r="V30" s="37"/>
-      <c r="W30" s="37"/>
-      <c r="X30" s="38"/>
-      <c r="Y30" s="38"/>
+      <c r="V30" s="41"/>
+      <c r="W30" s="41"/>
+      <c r="X30" s="40"/>
+      <c r="Y30" s="40"/>
       <c r="Z30" s="12"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
@@ -3695,14 +3809,14 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V31" s="37" t="s">
-        <v>229</v>
-      </c>
-      <c r="W31" s="37"/>
-      <c r="X31" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="Y31" s="38"/>
+      <c r="V31" s="41" t="s">
+        <v>225</v>
+      </c>
+      <c r="W31" s="41"/>
+      <c r="X31" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y31" s="40"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
@@ -3752,10 +3866,10 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="V32" s="37"/>
-      <c r="W32" s="37"/>
-      <c r="X32" s="38"/>
-      <c r="Y32" s="38"/>
+      <c r="V32" s="41"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="40"/>
+      <c r="Y32" s="40"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
@@ -3805,10 +3919,10 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="V33" s="37"/>
-      <c r="W33" s="37"/>
-      <c r="X33" s="38"/>
-      <c r="Y33" s="38"/>
+      <c r="V33" s="41"/>
+      <c r="W33" s="41"/>
+      <c r="X33" s="40"/>
+      <c r="Y33" s="40"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
@@ -3858,14 +3972,14 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="V34" s="37" t="s">
+      <c r="V34" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="W34" s="37"/>
-      <c r="X34" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y34" s="38"/>
+      <c r="W34" s="41"/>
+      <c r="X34" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y34" s="40"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
@@ -3917,10 +4031,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V35" s="37"/>
-      <c r="W35" s="37"/>
-      <c r="X35" s="38"/>
-      <c r="Y35" s="38"/>
+      <c r="V35" s="41"/>
+      <c r="W35" s="41"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="40"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
@@ -3972,10 +4086,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V36" s="37"/>
-      <c r="W36" s="37"/>
-      <c r="X36" s="38"/>
-      <c r="Y36" s="38"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="41"/>
+      <c r="X36" s="40"/>
+      <c r="Y36" s="40"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
@@ -6463,8 +6577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6504,14 +6618,14 @@
       <c r="G1" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="44" t="s">
-        <v>236</v>
+      <c r="H1" s="47" t="s">
+        <v>232</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6533,12 +6647,12 @@
       <c r="G2" s="29">
         <v>1634.7323951118842</v>
       </c>
-      <c r="H2" s="45"/>
+      <c r="H2" s="48"/>
       <c r="I2" s="18" t="s">
         <v>36</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6560,12 +6674,12 @@
       <c r="G3" s="29">
         <v>1814.5249435617134</v>
       </c>
-      <c r="H3" s="45"/>
+      <c r="H3" s="48"/>
       <c r="I3" s="18" t="s">
         <v>22</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -6587,12 +6701,12 @@
       <c r="G4" s="29">
         <v>1328.2178546508412</v>
       </c>
-      <c r="H4" s="45"/>
+      <c r="H4" s="48"/>
       <c r="I4" s="18" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -6614,12 +6728,12 @@
       <c r="G5" s="29">
         <v>1964.4036484206181</v>
       </c>
-      <c r="H5" s="45"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="18" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -6641,12 +6755,12 @@
       <c r="G6" s="29">
         <v>2139.8956184298472</v>
       </c>
-      <c r="H6" s="45"/>
+      <c r="H6" s="48"/>
       <c r="I6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -6668,12 +6782,12 @@
       <c r="G7" s="29">
         <v>1629.264793136442</v>
       </c>
-      <c r="H7" s="45"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="18" t="s">
         <v>73</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -6695,12 +6809,12 @@
       <c r="G8" s="29">
         <v>904.89457458099537</v>
       </c>
-      <c r="H8" s="46"/>
+      <c r="H8" s="49"/>
       <c r="I8" s="18" t="s">
         <v>74</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -6781,7 +6895,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C2" sqref="C2:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6809,7 +6923,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>8</v>
@@ -6820,14 +6934,14 @@
       <c r="G1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="38" t="s">
-        <v>148</v>
+      <c r="H1" s="40" t="s">
+        <v>145</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6852,12 +6966,12 @@
       <c r="G2" s="17">
         <v>118</v>
       </c>
-      <c r="H2" s="38"/>
+      <c r="H2" s="40"/>
       <c r="I2" s="18" t="s">
         <v>36</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6882,12 +6996,12 @@
       <c r="G3" s="17">
         <v>5</v>
       </c>
-      <c r="H3" s="38"/>
+      <c r="H3" s="40"/>
       <c r="I3" s="18" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -6912,14 +7026,14 @@
       <c r="G4" s="17">
         <v>5</v>
       </c>
-      <c r="H4" s="38" t="s">
-        <v>149</v>
+      <c r="H4" s="40" t="s">
+        <v>146</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -6944,12 +7058,12 @@
       <c r="G5" s="17">
         <v>9</v>
       </c>
-      <c r="H5" s="38"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -6974,12 +7088,12 @@
       <c r="G6" s="17">
         <v>7</v>
       </c>
-      <c r="H6" s="38"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="18" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -7008,7 +7122,7 @@
         <v>48</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -7037,7 +7151,7 @@
         <v>53</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -7687,13 +7801,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D39" s="16">
         <v>1</v>
@@ -7723,14 +7837,14 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D1" sqref="D1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="58.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="92.33203125" style="1" customWidth="1"/>
   </cols>
@@ -7746,10 +7860,10 @@
         <v>77</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -7794,13 +7908,13 @@
         <v>39</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>77</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -7824,7 +7938,7 @@
         <v>92</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>101</v>
+        <v>234</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
@@ -7837,7 +7951,7 @@
         <v>93</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -7850,7 +7964,7 @@
         <v>94</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -7863,7 +7977,7 @@
         <v>95</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>103</v>
+        <v>233</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -7876,7 +7990,7 @@
         <v>96</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>105</v>
+        <v>235</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -7889,7 +8003,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
@@ -7902,7 +8016,7 @@
         <v>97</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>162</v>
+        <v>236</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -7913,6 +8027,273 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFCD204-8EEA-41CE-94A6-48833B4F60E9}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="119.44140625" style="17" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="17">
+        <v>768.2</v>
+      </c>
+      <c r="C2" s="17">
+        <v>10</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" s="17">
+        <v>895.7</v>
+      </c>
+      <c r="C3" s="17">
+        <v>10</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1217.5</v>
+      </c>
+      <c r="C4" s="17">
+        <v>10</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1042.8</v>
+      </c>
+      <c r="C5" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1357.2</v>
+      </c>
+      <c r="C6" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1373.3</v>
+      </c>
+      <c r="C7" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1196.8</v>
+      </c>
+      <c r="C8" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="17">
+        <v>1522.3</v>
+      </c>
+      <c r="C9" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1350.6</v>
+      </c>
+      <c r="C10" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1665.6</v>
+      </c>
+      <c r="C11" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="B12" s="17">
+        <v>1816.6</v>
+      </c>
+      <c r="C12" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="B13" s="17">
+        <v>2000.3</v>
+      </c>
+      <c r="C13" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="17">
+        <v>1786.4</v>
+      </c>
+      <c r="C14" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" s="17">
+        <v>2243.6</v>
+      </c>
+      <c r="C15" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" s="17">
+        <v>2575.6</v>
+      </c>
+      <c r="C16" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" s="17">
+        <v>3034.2</v>
+      </c>
+      <c r="C17" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" s="17">
+        <v>40.1</v>
+      </c>
+      <c r="C18" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" s="17">
+        <v>89.9</v>
+      </c>
+      <c r="C19" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="B20" s="17">
+        <v>139.6</v>
+      </c>
+      <c r="C20" s="17">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDBEAB1-8D74-44E1-B064-2F1BCE93660D}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -7941,22 +8322,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -7982,7 +8363,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -8002,7 +8383,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8019,10 +8400,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -8039,15 +8420,15 @@
         <v>3</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>4</v>
@@ -8059,10 +8440,10 @@
         <v>3</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -8079,10 +8460,10 @@
         <v>3</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -8143,7 +8524,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>4</v>
@@ -8157,7 +8538,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>4</v>
@@ -8175,12 +8556,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1D9863-0B75-4A54-BECC-533A542694F0}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8195,218 +8576,229 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>113</v>
+        <v>261</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>107</v>
+        <v>262</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>194</v>
+        <v>263</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>77</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>217</v>
+        <v>112</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
-        <v>116</v>
+        <v>213</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="33">
-        <v>3000</v>
+        <v>114</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>108</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>189</v>
+        <v>115</v>
+      </c>
+      <c r="B9" s="33">
+        <v>3000</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>111</v>
+        <v>187</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
-        <v>187</v>
+        <v>182</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>108</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>192</v>
+        <v>109</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>209</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on adding user instructions...
</commit_message>
<xml_diff>
--- a/GCIRMS_Processor/GCIRMS Template.xlsx
+++ b/GCIRMS_Processor/GCIRMS Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13481491-5DA0-4335-86D4-CC3F8D643B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2565DB57-6283-4A24-8ABC-63343B6D4D7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1528,10 +1528,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2735,7 +2735,7 @@
         <v>58.75</v>
       </c>
       <c r="S13" s="10"/>
-      <c r="T13" s="40" t="s">
+      <c r="T13" s="41" t="s">
         <v>135</v>
       </c>
       <c r="U13" s="11"/>
@@ -2800,7 +2800,7 @@
         <v>40.35</v>
       </c>
       <c r="S14" s="10"/>
-      <c r="T14" s="40"/>
+      <c r="T14" s="41"/>
       <c r="U14" s="11"/>
       <c r="V14" s="45"/>
       <c r="W14" s="45"/>
@@ -2859,7 +2859,7 @@
         <v>40.35</v>
       </c>
       <c r="S15" s="10"/>
-      <c r="T15" s="40"/>
+      <c r="T15" s="41"/>
       <c r="U15" s="11"/>
       <c r="V15" s="45"/>
       <c r="W15" s="45"/>
@@ -2918,18 +2918,18 @@
         <v>40.35</v>
       </c>
       <c r="S16" s="10"/>
-      <c r="T16" s="40" t="s">
+      <c r="T16" s="41" t="s">
         <v>129</v>
       </c>
       <c r="U16" s="11"/>
-      <c r="V16" s="41" t="s">
+      <c r="V16" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="W16" s="41"/>
-      <c r="X16" s="40" t="s">
+      <c r="W16" s="40"/>
+      <c r="X16" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="Y16" s="40"/>
+      <c r="Y16" s="41"/>
       <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -2983,12 +2983,12 @@
         <v>40.35</v>
       </c>
       <c r="S17" s="10"/>
-      <c r="T17" s="40"/>
+      <c r="T17" s="41"/>
       <c r="U17" s="11"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="40"/>
-      <c r="Y17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="40"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="41"/>
       <c r="Z17" s="12"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -3042,12 +3042,12 @@
         <v>40.35</v>
       </c>
       <c r="S18" s="10"/>
-      <c r="T18" s="40"/>
+      <c r="T18" s="41"/>
       <c r="U18" s="11"/>
-      <c r="V18" s="41"/>
-      <c r="W18" s="41"/>
-      <c r="X18" s="40"/>
-      <c r="Y18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41"/>
       <c r="Z18" s="12"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
@@ -3101,18 +3101,18 @@
         <v>40.35</v>
       </c>
       <c r="S19" s="10"/>
-      <c r="T19" s="40" t="s">
+      <c r="T19" s="41" t="s">
         <v>130</v>
       </c>
       <c r="U19" s="11"/>
-      <c r="V19" s="41" t="s">
+      <c r="V19" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="W19" s="41"/>
-      <c r="X19" s="40" t="s">
+      <c r="W19" s="40"/>
+      <c r="X19" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="Y19" s="40"/>
+      <c r="Y19" s="41"/>
       <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -3166,12 +3166,12 @@
         <v>40.35</v>
       </c>
       <c r="S20" s="10"/>
-      <c r="T20" s="40"/>
+      <c r="T20" s="41"/>
       <c r="U20" s="11"/>
-      <c r="V20" s="41"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="40"/>
-      <c r="Y20" s="40"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="40"/>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="41"/>
       <c r="Z20" s="12"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -3225,12 +3225,12 @@
         <v>40.35</v>
       </c>
       <c r="S21" s="10"/>
-      <c r="T21" s="40"/>
+      <c r="T21" s="41"/>
       <c r="U21" s="11"/>
-      <c r="V21" s="41"/>
-      <c r="W21" s="41"/>
-      <c r="X21" s="40"/>
-      <c r="Y21" s="40"/>
+      <c r="V21" s="40"/>
+      <c r="W21" s="40"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="41"/>
       <c r="Z21" s="12"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
@@ -3283,18 +3283,18 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T22" s="40" t="s">
+      <c r="T22" s="41" t="s">
         <v>138</v>
       </c>
       <c r="U22" s="10"/>
-      <c r="V22" s="41" t="s">
+      <c r="V22" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="W22" s="41"/>
-      <c r="X22" s="40" t="s">
+      <c r="W22" s="40"/>
+      <c r="X22" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="Y22" s="40"/>
+      <c r="Y22" s="41"/>
       <c r="Z22" s="12"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -3347,12 +3347,12 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T23" s="40"/>
+      <c r="T23" s="41"/>
       <c r="U23" s="10"/>
-      <c r="V23" s="41"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="40"/>
-      <c r="Y23" s="40"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="40"/>
+      <c r="X23" s="41"/>
+      <c r="Y23" s="41"/>
       <c r="Z23" s="12"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -3403,12 +3403,12 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="T24" s="40"/>
+      <c r="T24" s="41"/>
       <c r="U24" s="10"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="40"/>
-      <c r="Y24" s="40"/>
+      <c r="V24" s="40"/>
+      <c r="W24" s="40"/>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="41"/>
       <c r="Z24" s="12"/>
     </row>
     <row r="25" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3463,14 +3463,14 @@
         <v>132</v>
       </c>
       <c r="U25" s="10"/>
-      <c r="V25" s="41" t="s">
+      <c r="V25" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="W25" s="41"/>
-      <c r="X25" s="40" t="s">
+      <c r="W25" s="40"/>
+      <c r="X25" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="Y25" s="40"/>
+      <c r="Y25" s="41"/>
       <c r="Z25" s="12"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3523,10 +3523,10 @@
       </c>
       <c r="T26" s="43"/>
       <c r="U26" s="10"/>
-      <c r="V26" s="41"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="40"/>
-      <c r="Y26" s="40"/>
+      <c r="V26" s="40"/>
+      <c r="W26" s="40"/>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="41"/>
       <c r="Z26" s="12"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -3579,10 +3579,10 @@
       </c>
       <c r="T27" s="43"/>
       <c r="U27" s="10"/>
-      <c r="V27" s="41"/>
-      <c r="W27" s="41"/>
-      <c r="X27" s="40"/>
-      <c r="Y27" s="40"/>
+      <c r="V27" s="40"/>
+      <c r="W27" s="40"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41"/>
       <c r="Z27" s="12"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
@@ -3635,14 +3635,14 @@
       </c>
       <c r="T28" s="43"/>
       <c r="U28" s="10"/>
-      <c r="V28" s="41" t="s">
+      <c r="V28" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="W28" s="41"/>
-      <c r="X28" s="40" t="s">
+      <c r="W28" s="40"/>
+      <c r="X28" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="Y28" s="40"/>
+      <c r="Y28" s="41"/>
       <c r="Z28" s="12"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -3695,10 +3695,10 @@
       </c>
       <c r="T29" s="43"/>
       <c r="U29" s="10"/>
-      <c r="V29" s="41"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="40"/>
-      <c r="Y29" s="40"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="40"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41"/>
       <c r="Z29" s="12"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -3753,10 +3753,10 @@
       </c>
       <c r="T30" s="44"/>
       <c r="U30" s="10"/>
-      <c r="V30" s="41"/>
-      <c r="W30" s="41"/>
-      <c r="X30" s="40"/>
-      <c r="Y30" s="40"/>
+      <c r="V30" s="40"/>
+      <c r="W30" s="40"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="41"/>
       <c r="Z30" s="12"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
@@ -3809,14 +3809,14 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V31" s="41" t="s">
+      <c r="V31" s="40" t="s">
         <v>225</v>
       </c>
-      <c r="W31" s="41"/>
-      <c r="X31" s="40" t="s">
+      <c r="W31" s="40"/>
+      <c r="X31" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="Y31" s="40"/>
+      <c r="Y31" s="41"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
@@ -3866,10 +3866,10 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="V32" s="41"/>
-      <c r="W32" s="41"/>
-      <c r="X32" s="40"/>
-      <c r="Y32" s="40"/>
+      <c r="V32" s="40"/>
+      <c r="W32" s="40"/>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="41"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
@@ -3919,10 +3919,10 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="V33" s="41"/>
-      <c r="W33" s="41"/>
-      <c r="X33" s="40"/>
-      <c r="Y33" s="40"/>
+      <c r="V33" s="40"/>
+      <c r="W33" s="40"/>
+      <c r="X33" s="41"/>
+      <c r="Y33" s="41"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
@@ -3972,14 +3972,14 @@
         <f t="shared" si="2"/>
         <v>58.75</v>
       </c>
-      <c r="V34" s="41" t="s">
+      <c r="V34" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="W34" s="41"/>
-      <c r="X34" s="40" t="s">
+      <c r="W34" s="40"/>
+      <c r="X34" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="Y34" s="40"/>
+      <c r="Y34" s="41"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
@@ -4031,10 +4031,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V35" s="41"/>
-      <c r="W35" s="41"/>
-      <c r="X35" s="40"/>
-      <c r="Y35" s="40"/>
+      <c r="V35" s="40"/>
+      <c r="W35" s="40"/>
+      <c r="X35" s="41"/>
+      <c r="Y35" s="41"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
@@ -4086,10 +4086,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V36" s="41"/>
-      <c r="W36" s="41"/>
-      <c r="X36" s="40"/>
-      <c r="Y36" s="40"/>
+      <c r="V36" s="40"/>
+      <c r="W36" s="40"/>
+      <c r="X36" s="41"/>
+      <c r="Y36" s="41"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
@@ -6545,6 +6545,11 @@
     <sortCondition descending="1" ref="A41:A46"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="X22:Y24"/>
+    <mergeCell ref="V25:W27"/>
+    <mergeCell ref="X25:Y27"/>
+    <mergeCell ref="V28:W30"/>
+    <mergeCell ref="X28:Y30"/>
     <mergeCell ref="V34:W36"/>
     <mergeCell ref="X34:Y36"/>
     <mergeCell ref="T13:T15"/>
@@ -6561,11 +6566,6 @@
     <mergeCell ref="V31:W33"/>
     <mergeCell ref="X31:Y33"/>
     <mergeCell ref="V22:W24"/>
-    <mergeCell ref="X22:Y24"/>
-    <mergeCell ref="V25:W27"/>
-    <mergeCell ref="X25:Y27"/>
-    <mergeCell ref="V28:W30"/>
-    <mergeCell ref="X28:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6934,7 +6934,7 @@
       <c r="G1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="41" t="s">
         <v>145</v>
       </c>
       <c r="I1" s="19" t="s">
@@ -6966,7 +6966,7 @@
       <c r="G2" s="17">
         <v>118</v>
       </c>
-      <c r="H2" s="40"/>
+      <c r="H2" s="41"/>
       <c r="I2" s="18" t="s">
         <v>36</v>
       </c>
@@ -6996,7 +6996,7 @@
       <c r="G3" s="17">
         <v>5</v>
       </c>
-      <c r="H3" s="40"/>
+      <c r="H3" s="41"/>
       <c r="I3" s="18" t="s">
         <v>11</v>
       </c>
@@ -7026,7 +7026,7 @@
       <c r="G4" s="17">
         <v>5</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="41" t="s">
         <v>146</v>
       </c>
       <c r="I4" s="18" t="s">
@@ -7058,7 +7058,7 @@
       <c r="G5" s="17">
         <v>9</v>
       </c>
-      <c r="H5" s="40"/>
+      <c r="H5" s="41"/>
       <c r="I5" s="18" t="s">
         <v>131</v>
       </c>
@@ -7088,7 +7088,7 @@
       <c r="G6" s="17">
         <v>7</v>
       </c>
-      <c r="H6" s="40"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="18" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
More in-app instructions. Raw IRMS can now be CSV, XLS, or XLSX.
</commit_message>
<xml_diff>
--- a/GCIRMS_Processor/GCIRMS Template.xlsx
+++ b/GCIRMS_Processor/GCIRMS Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C56115-E39B-4A15-943B-C0F110255FA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFB2A55-572A-446A-B1B7-2FC808956D6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="273">
   <si>
     <t>id1</t>
   </si>
@@ -1223,6 +1223,9 @@
   </si>
   <si>
     <t>H2 60m 6C_ramp Phthalic_Acid.met</t>
+  </si>
+  <si>
+    <t>comp_class</t>
   </si>
 </sst>
 </file>
@@ -1623,7 +1626,40 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1635,10 +1671,31 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1648,22 +1705,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1671,49 +1716,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2108,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2313,7 +2316,7 @@
         <v>H2 60m 6C_ramp Phthalic_Acid.met</v>
       </c>
       <c r="Q3" s="6">
-        <f t="shared" ref="Q3:Q66" si="2">INDEX(V$2:V$4,MATCH(O3,U$2:U$4,0))</f>
+        <f t="shared" ref="Q3:Q53" si="2">INDEX(V$2:V$4,MATCH(O3,U$2:U$4,0))</f>
         <v>14.82</v>
       </c>
       <c r="S3" s="7" t="s">
@@ -2866,18 +2869,18 @@
         <v>14.82</v>
       </c>
       <c r="S13" s="9"/>
-      <c r="T13" s="39" t="s">
+      <c r="T13" s="50" t="s">
         <v>132</v>
       </c>
       <c r="U13" s="10"/>
-      <c r="V13" s="42" t="s">
+      <c r="V13" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="W13" s="43"/>
-      <c r="X13" s="44" t="s">
+      <c r="W13" s="57"/>
+      <c r="X13" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="Y13" s="45"/>
+      <c r="Y13" s="63"/>
       <c r="Z13" s="11"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -2931,12 +2934,12 @@
         <v>14.82</v>
       </c>
       <c r="S14" s="9"/>
-      <c r="T14" s="40"/>
+      <c r="T14" s="51"/>
       <c r="U14" s="10"/>
-      <c r="V14" s="46"/>
-      <c r="W14" s="47"/>
-      <c r="X14" s="48"/>
-      <c r="Y14" s="49"/>
+      <c r="V14" s="58"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="64"/>
+      <c r="Y14" s="65"/>
       <c r="Z14" s="11"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -2990,12 +2993,12 @@
         <v>14.82</v>
       </c>
       <c r="S15" s="9"/>
-      <c r="T15" s="41"/>
+      <c r="T15" s="52"/>
       <c r="U15" s="10"/>
-      <c r="V15" s="50"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="52"/>
-      <c r="Y15" s="53"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="61"/>
+      <c r="X15" s="66"/>
+      <c r="Y15" s="67"/>
       <c r="Z15" s="11"/>
     </row>
     <row r="16" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3049,18 +3052,18 @@
         <v>14.82</v>
       </c>
       <c r="S16" s="9"/>
-      <c r="T16" s="39" t="s">
+      <c r="T16" s="50" t="s">
         <v>126</v>
       </c>
       <c r="U16" s="10"/>
-      <c r="V16" s="54" t="s">
+      <c r="V16" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="W16" s="55"/>
-      <c r="X16" s="56" t="s">
+      <c r="W16" s="39"/>
+      <c r="X16" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="Y16" s="57"/>
+      <c r="Y16" s="45"/>
       <c r="Z16" s="11"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -3114,12 +3117,12 @@
         <v>14.82</v>
       </c>
       <c r="S17" s="9"/>
-      <c r="T17" s="40"/>
+      <c r="T17" s="51"/>
       <c r="U17" s="10"/>
-      <c r="V17" s="58"/>
-      <c r="W17" s="59"/>
-      <c r="X17" s="60"/>
-      <c r="Y17" s="61"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="46"/>
+      <c r="Y17" s="47"/>
       <c r="Z17" s="11"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -3173,12 +3176,12 @@
         <v>14.82</v>
       </c>
       <c r="S18" s="9"/>
-      <c r="T18" s="41"/>
+      <c r="T18" s="52"/>
       <c r="U18" s="10"/>
-      <c r="V18" s="62"/>
-      <c r="W18" s="63"/>
-      <c r="X18" s="64"/>
-      <c r="Y18" s="65"/>
+      <c r="V18" s="42"/>
+      <c r="W18" s="43"/>
+      <c r="X18" s="48"/>
+      <c r="Y18" s="49"/>
       <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3232,18 +3235,18 @@
         <v>14.82</v>
       </c>
       <c r="S19" s="9"/>
-      <c r="T19" s="39" t="s">
+      <c r="T19" s="50" t="s">
         <v>127</v>
       </c>
       <c r="U19" s="10"/>
-      <c r="V19" s="54" t="s">
+      <c r="V19" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="W19" s="55"/>
-      <c r="X19" s="56" t="s">
+      <c r="W19" s="39"/>
+      <c r="X19" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="Y19" s="57"/>
+      <c r="Y19" s="45"/>
       <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -3297,12 +3300,12 @@
         <v>14.82</v>
       </c>
       <c r="S20" s="9"/>
-      <c r="T20" s="40"/>
+      <c r="T20" s="51"/>
       <c r="U20" s="10"/>
-      <c r="V20" s="58"/>
-      <c r="W20" s="59"/>
-      <c r="X20" s="60"/>
-      <c r="Y20" s="61"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="46"/>
+      <c r="Y20" s="47"/>
       <c r="Z20" s="11"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -3356,12 +3359,12 @@
         <v>14.82</v>
       </c>
       <c r="S21" s="9"/>
-      <c r="T21" s="41"/>
+      <c r="T21" s="52"/>
       <c r="U21" s="10"/>
-      <c r="V21" s="62"/>
-      <c r="W21" s="63"/>
-      <c r="X21" s="64"/>
-      <c r="Y21" s="65"/>
+      <c r="V21" s="42"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="48"/>
+      <c r="Y21" s="49"/>
       <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3414,18 +3417,18 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T22" s="39" t="s">
+      <c r="T22" s="50" t="s">
         <v>135</v>
       </c>
       <c r="U22" s="9"/>
-      <c r="V22" s="54" t="s">
+      <c r="V22" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="W22" s="55"/>
-      <c r="X22" s="56" t="s">
+      <c r="W22" s="39"/>
+      <c r="X22" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="Y22" s="57"/>
+      <c r="Y22" s="45"/>
       <c r="Z22" s="11"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -3478,12 +3481,12 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T23" s="40"/>
+      <c r="T23" s="51"/>
       <c r="U23" s="9"/>
-      <c r="V23" s="58"/>
-      <c r="W23" s="59"/>
-      <c r="X23" s="60"/>
-      <c r="Y23" s="61"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="41"/>
+      <c r="X23" s="46"/>
+      <c r="Y23" s="47"/>
       <c r="Z23" s="11"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -3536,12 +3539,12 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T24" s="41"/>
+      <c r="T24" s="52"/>
       <c r="U24" s="9"/>
-      <c r="V24" s="62"/>
-      <c r="W24" s="63"/>
-      <c r="X24" s="64"/>
-      <c r="Y24" s="65"/>
+      <c r="V24" s="42"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="48"/>
+      <c r="Y24" s="49"/>
       <c r="Z24" s="11"/>
     </row>
     <row r="25" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3594,18 +3597,18 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T25" s="66" t="s">
+      <c r="T25" s="53" t="s">
         <v>129</v>
       </c>
       <c r="U25" s="9"/>
-      <c r="V25" s="54" t="s">
+      <c r="V25" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="W25" s="55"/>
-      <c r="X25" s="56" t="s">
+      <c r="W25" s="39"/>
+      <c r="X25" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="Y25" s="57"/>
+      <c r="Y25" s="45"/>
       <c r="Z25" s="11"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3658,12 +3661,12 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T26" s="67"/>
+      <c r="T26" s="54"/>
       <c r="U26" s="9"/>
-      <c r="V26" s="58"/>
-      <c r="W26" s="59"/>
-      <c r="X26" s="60"/>
-      <c r="Y26" s="61"/>
+      <c r="V26" s="40"/>
+      <c r="W26" s="41"/>
+      <c r="X26" s="46"/>
+      <c r="Y26" s="47"/>
       <c r="Z26" s="11"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -3716,12 +3719,12 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T27" s="67"/>
+      <c r="T27" s="54"/>
       <c r="U27" s="9"/>
-      <c r="V27" s="62"/>
-      <c r="W27" s="63"/>
-      <c r="X27" s="64"/>
-      <c r="Y27" s="65"/>
+      <c r="V27" s="42"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="48"/>
+      <c r="Y27" s="49"/>
       <c r="Z27" s="11"/>
     </row>
     <row r="28" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3774,16 +3777,16 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T28" s="67"/>
+      <c r="T28" s="54"/>
       <c r="U28" s="9"/>
-      <c r="V28" s="54" t="s">
+      <c r="V28" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="W28" s="55"/>
-      <c r="X28" s="56" t="s">
+      <c r="W28" s="39"/>
+      <c r="X28" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="Y28" s="57"/>
+      <c r="Y28" s="45"/>
       <c r="Z28" s="11"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -3836,12 +3839,12 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T29" s="67"/>
+      <c r="T29" s="54"/>
       <c r="U29" s="9"/>
-      <c r="V29" s="58"/>
-      <c r="W29" s="59"/>
-      <c r="X29" s="60"/>
-      <c r="Y29" s="61"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="46"/>
+      <c r="Y29" s="47"/>
       <c r="Z29" s="11"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -3894,12 +3897,12 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="T30" s="68"/>
+      <c r="T30" s="55"/>
       <c r="U30" s="9"/>
-      <c r="V30" s="62"/>
-      <c r="W30" s="63"/>
-      <c r="X30" s="64"/>
-      <c r="Y30" s="65"/>
+      <c r="V30" s="42"/>
+      <c r="W30" s="43"/>
+      <c r="X30" s="48"/>
+      <c r="Y30" s="49"/>
       <c r="Z30" s="11"/>
     </row>
     <row r="31" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3952,14 +3955,14 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V31" s="54" t="s">
+      <c r="V31" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="W31" s="55"/>
-      <c r="X31" s="56" t="s">
+      <c r="W31" s="39"/>
+      <c r="X31" s="44" t="s">
         <v>222</v>
       </c>
-      <c r="Y31" s="57"/>
+      <c r="Y31" s="45"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
@@ -4011,10 +4014,10 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V32" s="58"/>
-      <c r="W32" s="59"/>
-      <c r="X32" s="60"/>
-      <c r="Y32" s="61"/>
+      <c r="V32" s="40"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="46"/>
+      <c r="Y32" s="47"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
@@ -4066,10 +4069,10 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V33" s="62"/>
-      <c r="W33" s="63"/>
-      <c r="X33" s="64"/>
-      <c r="Y33" s="65"/>
+      <c r="V33" s="42"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="48"/>
+      <c r="Y33" s="49"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
@@ -4121,14 +4124,14 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V34" s="54" t="s">
+      <c r="V34" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="W34" s="55"/>
-      <c r="X34" s="56" t="s">
+      <c r="W34" s="39"/>
+      <c r="X34" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="Y34" s="57"/>
+      <c r="Y34" s="45"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
@@ -4180,10 +4183,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V35" s="58"/>
-      <c r="W35" s="59"/>
-      <c r="X35" s="60"/>
-      <c r="Y35" s="61"/>
+      <c r="V35" s="40"/>
+      <c r="W35" s="41"/>
+      <c r="X35" s="46"/>
+      <c r="Y35" s="47"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
@@ -4235,10 +4238,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V36" s="62"/>
-      <c r="W36" s="63"/>
-      <c r="X36" s="64"/>
-      <c r="Y36" s="65"/>
+      <c r="V36" s="42"/>
+      <c r="W36" s="43"/>
+      <c r="X36" s="48"/>
+      <c r="Y36" s="49"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -6204,6 +6207,11 @@
     <sortCondition descending="1" ref="A41:A46"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="X22:Y24"/>
+    <mergeCell ref="V25:W27"/>
+    <mergeCell ref="X25:Y27"/>
+    <mergeCell ref="V28:W30"/>
+    <mergeCell ref="X28:Y30"/>
     <mergeCell ref="V34:W36"/>
     <mergeCell ref="X34:Y36"/>
     <mergeCell ref="T13:T15"/>
@@ -6220,11 +6228,6 @@
     <mergeCell ref="V31:W33"/>
     <mergeCell ref="X31:Y33"/>
     <mergeCell ref="V22:W24"/>
-    <mergeCell ref="X22:Y24"/>
-    <mergeCell ref="V25:W27"/>
-    <mergeCell ref="X25:Y27"/>
-    <mergeCell ref="V28:W30"/>
-    <mergeCell ref="X28:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6277,7 +6280,7 @@
       <c r="G1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="50" t="s">
         <v>228</v>
       </c>
       <c r="I1" s="17" t="s">
@@ -6306,7 +6309,7 @@
       <c r="G2" s="27">
         <v>1634.7323951118842</v>
       </c>
-      <c r="H2" s="40"/>
+      <c r="H2" s="51"/>
       <c r="I2" s="16" t="s">
         <v>36</v>
       </c>
@@ -6333,7 +6336,7 @@
       <c r="G3" s="27">
         <v>1814.5249435617134</v>
       </c>
-      <c r="H3" s="40"/>
+      <c r="H3" s="51"/>
       <c r="I3" s="16" t="s">
         <v>22</v>
       </c>
@@ -6360,7 +6363,7 @@
       <c r="G4" s="27">
         <v>1328.2178546508412</v>
       </c>
-      <c r="H4" s="40"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="16" t="s">
         <v>1</v>
       </c>
@@ -6387,7 +6390,7 @@
       <c r="G5" s="27">
         <v>1964.4036484206181</v>
       </c>
-      <c r="H5" s="40"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="16" t="s">
         <v>2</v>
       </c>
@@ -6414,7 +6417,7 @@
       <c r="G6" s="27">
         <v>2139.8956184298472</v>
       </c>
-      <c r="H6" s="40"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="16" t="s">
         <v>3</v>
       </c>
@@ -6441,7 +6444,7 @@
       <c r="G7" s="27">
         <v>1629.264793136442</v>
       </c>
-      <c r="H7" s="40"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="16" t="s">
         <v>72</v>
       </c>
@@ -6468,7 +6471,7 @@
       <c r="G8" s="27">
         <v>904.89457458099537</v>
       </c>
-      <c r="H8" s="41"/>
+      <c r="H8" s="52"/>
       <c r="I8" s="16" t="s">
         <v>73</v>
       </c>
@@ -6553,8 +6556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6575,11 +6578,11 @@
       <c r="A1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>7</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>128</v>
@@ -6593,7 +6596,7 @@
       <c r="G1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="68" t="s">
         <v>141</v>
       </c>
       <c r="I1" s="17" t="s">
@@ -6608,10 +6611,10 @@
         <v>54</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="14">
         <v>1</v>
@@ -6625,7 +6628,7 @@
       <c r="G2" s="15">
         <v>118</v>
       </c>
-      <c r="H2" s="38"/>
+      <c r="H2" s="68"/>
       <c r="I2" s="16" t="s">
         <v>36</v>
       </c>
@@ -6638,10 +6641,10 @@
         <v>54</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="14">
         <v>1</v>
@@ -6655,7 +6658,7 @@
       <c r="G3" s="15">
         <v>5</v>
       </c>
-      <c r="H3" s="38"/>
+      <c r="H3" s="68"/>
       <c r="I3" s="16" t="s">
         <v>11</v>
       </c>
@@ -6668,10 +6671,10 @@
         <v>54</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>19</v>
       </c>
       <c r="D4" s="14">
         <v>1</v>
@@ -6685,7 +6688,7 @@
       <c r="G4" s="15">
         <v>5</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="68" t="s">
         <v>142</v>
       </c>
       <c r="I4" s="16" t="s">
@@ -6700,10 +6703,10 @@
         <v>54</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>55</v>
       </c>
       <c r="D5" s="14">
         <v>1</v>
@@ -6717,7 +6720,7 @@
       <c r="G5" s="15">
         <v>9</v>
       </c>
-      <c r="H5" s="38"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="16" t="s">
         <v>128</v>
       </c>
@@ -6730,10 +6733,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>14</v>
       </c>
       <c r="D6" s="14">
         <v>1</v>
@@ -6747,7 +6750,7 @@
       <c r="G6" s="15">
         <v>7</v>
       </c>
-      <c r="H6" s="38"/>
+      <c r="H6" s="68"/>
       <c r="I6" s="16" t="s">
         <v>8</v>
       </c>
@@ -6760,10 +6763,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="14">
         <v>1</v>
@@ -6789,10 +6792,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>16</v>
       </c>
       <c r="D8" s="14">
         <v>1</v>
@@ -6818,10 +6821,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>17</v>
       </c>
       <c r="D9" s="14">
         <v>1</v>
@@ -6841,10 +6844,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>18</v>
       </c>
       <c r="D10" s="14">
         <v>1</v>
@@ -6864,10 +6867,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>19</v>
       </c>
       <c r="D11" s="14">
         <v>1</v>
@@ -6878,10 +6881,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>20</v>
       </c>
       <c r="D12" s="14">
         <v>1</v>
@@ -6892,10 +6895,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="D13" s="14">
         <v>1</v>
@@ -6906,10 +6909,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>5</v>
       </c>
       <c r="D14" s="14">
         <v>1</v>
@@ -6920,10 +6923,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>6</v>
       </c>
       <c r="D15" s="14">
         <v>1</v>
@@ -6934,10 +6937,10 @@
         <v>43</v>
       </c>
       <c r="B16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="D16" s="14">
         <v>1</v>
@@ -6957,10 +6960,10 @@
         <v>43</v>
       </c>
       <c r="B17" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="D17" s="14">
         <v>1</v>
@@ -6980,10 +6983,10 @@
         <v>43</v>
       </c>
       <c r="B18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>46</v>
       </c>
       <c r="D18" s="14">
         <v>1</v>
@@ -7003,10 +7006,10 @@
         <v>43</v>
       </c>
       <c r="B19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>46</v>
       </c>
       <c r="D19" s="14">
         <v>1</v>
@@ -7026,10 +7029,10 @@
         <v>43</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>47</v>
       </c>
       <c r="D20" s="14">
         <v>1</v>
@@ -7049,10 +7052,10 @@
         <v>43</v>
       </c>
       <c r="B21" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>47</v>
       </c>
       <c r="D21" s="14">
         <v>1</v>
@@ -7072,10 +7075,10 @@
         <v>43</v>
       </c>
       <c r="B22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>13</v>
       </c>
       <c r="D22" s="14">
         <v>1</v>
@@ -7095,10 +7098,10 @@
         <v>43</v>
       </c>
       <c r="B23" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>13</v>
       </c>
       <c r="D23" s="14">
         <v>1</v>
@@ -7118,10 +7121,10 @@
         <v>49</v>
       </c>
       <c r="B24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>46</v>
       </c>
       <c r="D24" s="14">
         <v>1</v>
@@ -7141,10 +7144,10 @@
         <v>49</v>
       </c>
       <c r="B25" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>14</v>
       </c>
       <c r="D25" s="14">
         <v>1</v>
@@ -7164,10 +7167,10 @@
         <v>49</v>
       </c>
       <c r="B26" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>47</v>
       </c>
       <c r="D26" s="14">
         <v>1</v>
@@ -7187,10 +7190,10 @@
         <v>49</v>
       </c>
       <c r="B27" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>15</v>
       </c>
       <c r="D27" s="14">
         <v>1</v>
@@ -7210,10 +7213,10 @@
         <v>49</v>
       </c>
       <c r="B28" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>13</v>
       </c>
       <c r="D28" s="14">
         <v>1</v>
@@ -7233,10 +7236,10 @@
         <v>49</v>
       </c>
       <c r="B29" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>16</v>
       </c>
       <c r="D29" s="14">
         <v>1</v>
@@ -7256,10 +7259,10 @@
         <v>49</v>
       </c>
       <c r="B30" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="D30" s="14">
         <v>1</v>
@@ -7279,10 +7282,10 @@
         <v>49</v>
       </c>
       <c r="B31" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>17</v>
       </c>
       <c r="D31" s="14">
         <v>1</v>
@@ -7302,10 +7305,10 @@
         <v>49</v>
       </c>
       <c r="B32" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>19</v>
       </c>
       <c r="D32" s="14">
         <v>1</v>
@@ -7325,10 +7328,10 @@
         <v>49</v>
       </c>
       <c r="B33" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>18</v>
       </c>
       <c r="D33" s="14">
         <v>1</v>
@@ -7348,10 +7351,10 @@
         <v>49</v>
       </c>
       <c r="B34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>20</v>
       </c>
       <c r="D34" s="14">
         <v>1</v>
@@ -7371,10 +7374,10 @@
         <v>49</v>
       </c>
       <c r="B35" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>51</v>
       </c>
       <c r="D35" s="14">
         <v>1</v>
@@ -7394,10 +7397,10 @@
         <v>49</v>
       </c>
       <c r="B36" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="D36" s="14">
         <v>1</v>
@@ -7417,10 +7420,10 @@
         <v>49</v>
       </c>
       <c r="B37" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>52</v>
       </c>
       <c r="D37" s="14">
         <v>1</v>
@@ -7440,10 +7443,10 @@
         <v>49</v>
       </c>
       <c r="B38" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>5</v>
       </c>
       <c r="D38" s="14">
         <v>1</v>
@@ -7463,10 +7466,10 @@
         <v>223</v>
       </c>
       <c r="B39" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>224</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>225</v>
       </c>
       <c r="D39" s="14">
         <v>1</v>
@@ -7690,7 +7693,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7705,7 +7708,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>7</v>
+        <v>272</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>86</v>
@@ -7731,7 +7734,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>7</v>
+        <v>272</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>251</v>

</xml_diff>

<commit_message>
Development of derivative hydrogen correction. Still needs some UI polishing and the uncertainty calculation seems wrong.
</commit_message>
<xml_diff>
--- a/GCIRMS_Processor/GCIRMS Template.xlsx
+++ b/GCIRMS_Processor/GCIRMS Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFB2A55-572A-446A-B1B7-2FC808956D6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79F7354-325C-4D57-971E-963F0DBA633D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="276">
   <si>
     <t>id1</t>
   </si>
@@ -1226,6 +1226,15 @@
   </si>
   <si>
     <t>comp_class</t>
+  </si>
+  <si>
+    <t>derivatization_option</t>
+  </si>
+  <si>
+    <t>Template-defined derivative \u03B4D.</t>
+  </si>
+  <si>
+    <t>Choose where to source the δD of the derivative hydrogen.</t>
   </si>
 </sst>
 </file>
@@ -1627,6 +1636,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1643,24 +1670,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3056,14 +3065,14 @@
         <v>126</v>
       </c>
       <c r="U16" s="10"/>
-      <c r="V16" s="38" t="s">
+      <c r="V16" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="W16" s="39"/>
-      <c r="X16" s="44" t="s">
+      <c r="W16" s="45"/>
+      <c r="X16" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="Y16" s="45"/>
+      <c r="Y16" s="39"/>
       <c r="Z16" s="11"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -3119,10 +3128,10 @@
       <c r="S17" s="9"/>
       <c r="T17" s="51"/>
       <c r="U17" s="10"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="46"/>
-      <c r="Y17" s="47"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="40"/>
+      <c r="Y17" s="41"/>
       <c r="Z17" s="11"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -3178,10 +3187,10 @@
       <c r="S18" s="9"/>
       <c r="T18" s="52"/>
       <c r="U18" s="10"/>
-      <c r="V18" s="42"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="48"/>
-      <c r="Y18" s="49"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="43"/>
       <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3239,14 +3248,14 @@
         <v>127</v>
       </c>
       <c r="U19" s="10"/>
-      <c r="V19" s="38" t="s">
+      <c r="V19" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="W19" s="39"/>
-      <c r="X19" s="44" t="s">
+      <c r="W19" s="45"/>
+      <c r="X19" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="Y19" s="45"/>
+      <c r="Y19" s="39"/>
       <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -3302,10 +3311,10 @@
       <c r="S20" s="9"/>
       <c r="T20" s="51"/>
       <c r="U20" s="10"/>
-      <c r="V20" s="40"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="46"/>
-      <c r="Y20" s="47"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="47"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="41"/>
       <c r="Z20" s="11"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -3361,10 +3370,10 @@
       <c r="S21" s="9"/>
       <c r="T21" s="52"/>
       <c r="U21" s="10"/>
-      <c r="V21" s="42"/>
-      <c r="W21" s="43"/>
-      <c r="X21" s="48"/>
-      <c r="Y21" s="49"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="49"/>
+      <c r="X21" s="42"/>
+      <c r="Y21" s="43"/>
       <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3421,14 +3430,14 @@
         <v>135</v>
       </c>
       <c r="U22" s="9"/>
-      <c r="V22" s="38" t="s">
+      <c r="V22" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="W22" s="39"/>
-      <c r="X22" s="44" t="s">
+      <c r="W22" s="45"/>
+      <c r="X22" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="Y22" s="45"/>
+      <c r="Y22" s="39"/>
       <c r="Z22" s="11"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -3483,10 +3492,10 @@
       </c>
       <c r="T23" s="51"/>
       <c r="U23" s="9"/>
-      <c r="V23" s="40"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="46"/>
-      <c r="Y23" s="47"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="47"/>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="41"/>
       <c r="Z23" s="11"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -3541,10 +3550,10 @@
       </c>
       <c r="T24" s="52"/>
       <c r="U24" s="9"/>
-      <c r="V24" s="42"/>
-      <c r="W24" s="43"/>
-      <c r="X24" s="48"/>
-      <c r="Y24" s="49"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="49"/>
+      <c r="X24" s="42"/>
+      <c r="Y24" s="43"/>
       <c r="Z24" s="11"/>
     </row>
     <row r="25" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3601,14 +3610,14 @@
         <v>129</v>
       </c>
       <c r="U25" s="9"/>
-      <c r="V25" s="38" t="s">
+      <c r="V25" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="W25" s="39"/>
-      <c r="X25" s="44" t="s">
+      <c r="W25" s="45"/>
+      <c r="X25" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="Y25" s="45"/>
+      <c r="Y25" s="39"/>
       <c r="Z25" s="11"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3663,10 +3672,10 @@
       </c>
       <c r="T26" s="54"/>
       <c r="U26" s="9"/>
-      <c r="V26" s="40"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="46"/>
-      <c r="Y26" s="47"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="40"/>
+      <c r="Y26" s="41"/>
       <c r="Z26" s="11"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -3721,10 +3730,10 @@
       </c>
       <c r="T27" s="54"/>
       <c r="U27" s="9"/>
-      <c r="V27" s="42"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="48"/>
-      <c r="Y27" s="49"/>
+      <c r="V27" s="48"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="42"/>
+      <c r="Y27" s="43"/>
       <c r="Z27" s="11"/>
     </row>
     <row r="28" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3779,14 +3788,14 @@
       </c>
       <c r="T28" s="54"/>
       <c r="U28" s="9"/>
-      <c r="V28" s="38" t="s">
+      <c r="V28" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="W28" s="39"/>
-      <c r="X28" s="44" t="s">
+      <c r="W28" s="45"/>
+      <c r="X28" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="Y28" s="45"/>
+      <c r="Y28" s="39"/>
       <c r="Z28" s="11"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -3841,10 +3850,10 @@
       </c>
       <c r="T29" s="54"/>
       <c r="U29" s="9"/>
-      <c r="V29" s="40"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="46"/>
-      <c r="Y29" s="47"/>
+      <c r="V29" s="46"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="41"/>
       <c r="Z29" s="11"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -3899,10 +3908,10 @@
       </c>
       <c r="T30" s="55"/>
       <c r="U30" s="9"/>
-      <c r="V30" s="42"/>
-      <c r="W30" s="43"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="49"/>
+      <c r="V30" s="48"/>
+      <c r="W30" s="49"/>
+      <c r="X30" s="42"/>
+      <c r="Y30" s="43"/>
       <c r="Z30" s="11"/>
     </row>
     <row r="31" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3955,14 +3964,14 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V31" s="38" t="s">
+      <c r="V31" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="W31" s="39"/>
-      <c r="X31" s="44" t="s">
+      <c r="W31" s="45"/>
+      <c r="X31" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="Y31" s="45"/>
+      <c r="Y31" s="39"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
@@ -4014,10 +4023,10 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V32" s="40"/>
-      <c r="W32" s="41"/>
-      <c r="X32" s="46"/>
-      <c r="Y32" s="47"/>
+      <c r="V32" s="46"/>
+      <c r="W32" s="47"/>
+      <c r="X32" s="40"/>
+      <c r="Y32" s="41"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
@@ -4069,10 +4078,10 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V33" s="42"/>
-      <c r="W33" s="43"/>
-      <c r="X33" s="48"/>
-      <c r="Y33" s="49"/>
+      <c r="V33" s="48"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="43"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
@@ -4124,14 +4133,14 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V34" s="38" t="s">
+      <c r="V34" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="W34" s="39"/>
-      <c r="X34" s="44" t="s">
+      <c r="W34" s="45"/>
+      <c r="X34" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="Y34" s="45"/>
+      <c r="Y34" s="39"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
@@ -4183,10 +4192,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V35" s="40"/>
-      <c r="W35" s="41"/>
-      <c r="X35" s="46"/>
-      <c r="Y35" s="47"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="47"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="41"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
@@ -4238,10 +4247,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V36" s="42"/>
-      <c r="W36" s="43"/>
-      <c r="X36" s="48"/>
-      <c r="Y36" s="49"/>
+      <c r="V36" s="48"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="43"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -6207,11 +6216,6 @@
     <sortCondition descending="1" ref="A41:A46"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="X22:Y24"/>
-    <mergeCell ref="V25:W27"/>
-    <mergeCell ref="X25:Y27"/>
-    <mergeCell ref="V28:W30"/>
-    <mergeCell ref="X28:Y30"/>
     <mergeCell ref="V34:W36"/>
     <mergeCell ref="X34:Y36"/>
     <mergeCell ref="T13:T15"/>
@@ -6228,6 +6232,11 @@
     <mergeCell ref="V31:W33"/>
     <mergeCell ref="X31:Y33"/>
     <mergeCell ref="V22:W24"/>
+    <mergeCell ref="X22:Y24"/>
+    <mergeCell ref="V25:W27"/>
+    <mergeCell ref="X25:Y27"/>
+    <mergeCell ref="V28:W30"/>
+    <mergeCell ref="X28:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6556,7 +6565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -7960,7 +7969,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8220,10 +8229,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1D9863-0B75-4A54-BECC-533A542694F0}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8463,6 +8472,17 @@
         <v>201</v>
       </c>
     </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Initital work on sample error propagation tab, still in progress.
</commit_message>
<xml_diff>
--- a/GCIRMS_Processor/GCIRMS Template.xlsx
+++ b/GCIRMS_Processor/GCIRMS Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79F7354-325C-4D57-971E-963F0DBA633D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881E2B33-43BB-4743-963F-CAE873971BAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -1636,6 +1636,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1652,24 +1670,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3065,14 +3065,14 @@
         <v>126</v>
       </c>
       <c r="U16" s="10"/>
-      <c r="V16" s="44" t="s">
+      <c r="V16" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="W16" s="45"/>
-      <c r="X16" s="38" t="s">
+      <c r="W16" s="39"/>
+      <c r="X16" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="Y16" s="39"/>
+      <c r="Y16" s="45"/>
       <c r="Z16" s="11"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -3128,10 +3128,10 @@
       <c r="S17" s="9"/>
       <c r="T17" s="51"/>
       <c r="U17" s="10"/>
-      <c r="V17" s="46"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="40"/>
-      <c r="Y17" s="41"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="46"/>
+      <c r="Y17" s="47"/>
       <c r="Z17" s="11"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -3187,10 +3187,10 @@
       <c r="S18" s="9"/>
       <c r="T18" s="52"/>
       <c r="U18" s="10"/>
-      <c r="V18" s="48"/>
-      <c r="W18" s="49"/>
-      <c r="X18" s="42"/>
-      <c r="Y18" s="43"/>
+      <c r="V18" s="42"/>
+      <c r="W18" s="43"/>
+      <c r="X18" s="48"/>
+      <c r="Y18" s="49"/>
       <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3248,14 +3248,14 @@
         <v>127</v>
       </c>
       <c r="U19" s="10"/>
-      <c r="V19" s="44" t="s">
+      <c r="V19" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="W19" s="45"/>
-      <c r="X19" s="38" t="s">
+      <c r="W19" s="39"/>
+      <c r="X19" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="Y19" s="39"/>
+      <c r="Y19" s="45"/>
       <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -3311,10 +3311,10 @@
       <c r="S20" s="9"/>
       <c r="T20" s="51"/>
       <c r="U20" s="10"/>
-      <c r="V20" s="46"/>
-      <c r="W20" s="47"/>
-      <c r="X20" s="40"/>
-      <c r="Y20" s="41"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="46"/>
+      <c r="Y20" s="47"/>
       <c r="Z20" s="11"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -3370,10 +3370,10 @@
       <c r="S21" s="9"/>
       <c r="T21" s="52"/>
       <c r="U21" s="10"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="49"/>
-      <c r="X21" s="42"/>
-      <c r="Y21" s="43"/>
+      <c r="V21" s="42"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="48"/>
+      <c r="Y21" s="49"/>
       <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3430,14 +3430,14 @@
         <v>135</v>
       </c>
       <c r="U22" s="9"/>
-      <c r="V22" s="44" t="s">
+      <c r="V22" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="W22" s="45"/>
-      <c r="X22" s="38" t="s">
+      <c r="W22" s="39"/>
+      <c r="X22" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="Y22" s="39"/>
+      <c r="Y22" s="45"/>
       <c r="Z22" s="11"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -3492,10 +3492,10 @@
       </c>
       <c r="T23" s="51"/>
       <c r="U23" s="9"/>
-      <c r="V23" s="46"/>
-      <c r="W23" s="47"/>
-      <c r="X23" s="40"/>
-      <c r="Y23" s="41"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="41"/>
+      <c r="X23" s="46"/>
+      <c r="Y23" s="47"/>
       <c r="Z23" s="11"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -3550,10 +3550,10 @@
       </c>
       <c r="T24" s="52"/>
       <c r="U24" s="9"/>
-      <c r="V24" s="48"/>
-      <c r="W24" s="49"/>
-      <c r="X24" s="42"/>
-      <c r="Y24" s="43"/>
+      <c r="V24" s="42"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="48"/>
+      <c r="Y24" s="49"/>
       <c r="Z24" s="11"/>
     </row>
     <row r="25" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3610,14 +3610,14 @@
         <v>129</v>
       </c>
       <c r="U25" s="9"/>
-      <c r="V25" s="44" t="s">
+      <c r="V25" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="W25" s="45"/>
-      <c r="X25" s="38" t="s">
+      <c r="W25" s="39"/>
+      <c r="X25" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="Y25" s="39"/>
+      <c r="Y25" s="45"/>
       <c r="Z25" s="11"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3672,10 +3672,10 @@
       </c>
       <c r="T26" s="54"/>
       <c r="U26" s="9"/>
-      <c r="V26" s="46"/>
-      <c r="W26" s="47"/>
-      <c r="X26" s="40"/>
-      <c r="Y26" s="41"/>
+      <c r="V26" s="40"/>
+      <c r="W26" s="41"/>
+      <c r="X26" s="46"/>
+      <c r="Y26" s="47"/>
       <c r="Z26" s="11"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -3730,10 +3730,10 @@
       </c>
       <c r="T27" s="54"/>
       <c r="U27" s="9"/>
-      <c r="V27" s="48"/>
-      <c r="W27" s="49"/>
-      <c r="X27" s="42"/>
-      <c r="Y27" s="43"/>
+      <c r="V27" s="42"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="48"/>
+      <c r="Y27" s="49"/>
       <c r="Z27" s="11"/>
     </row>
     <row r="28" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3788,14 +3788,14 @@
       </c>
       <c r="T28" s="54"/>
       <c r="U28" s="9"/>
-      <c r="V28" s="44" t="s">
+      <c r="V28" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="W28" s="45"/>
-      <c r="X28" s="38" t="s">
+      <c r="W28" s="39"/>
+      <c r="X28" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="Y28" s="39"/>
+      <c r="Y28" s="45"/>
       <c r="Z28" s="11"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -3850,10 +3850,10 @@
       </c>
       <c r="T29" s="54"/>
       <c r="U29" s="9"/>
-      <c r="V29" s="46"/>
-      <c r="W29" s="47"/>
-      <c r="X29" s="40"/>
-      <c r="Y29" s="41"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="46"/>
+      <c r="Y29" s="47"/>
       <c r="Z29" s="11"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -3908,10 +3908,10 @@
       </c>
       <c r="T30" s="55"/>
       <c r="U30" s="9"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="49"/>
-      <c r="X30" s="42"/>
-      <c r="Y30" s="43"/>
+      <c r="V30" s="42"/>
+      <c r="W30" s="43"/>
+      <c r="X30" s="48"/>
+      <c r="Y30" s="49"/>
       <c r="Z30" s="11"/>
     </row>
     <row r="31" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3964,14 +3964,14 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V31" s="44" t="s">
+      <c r="V31" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="W31" s="45"/>
-      <c r="X31" s="38" t="s">
+      <c r="W31" s="39"/>
+      <c r="X31" s="44" t="s">
         <v>222</v>
       </c>
-      <c r="Y31" s="39"/>
+      <c r="Y31" s="45"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
@@ -4023,10 +4023,10 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V32" s="46"/>
-      <c r="W32" s="47"/>
-      <c r="X32" s="40"/>
-      <c r="Y32" s="41"/>
+      <c r="V32" s="40"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="46"/>
+      <c r="Y32" s="47"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
@@ -4078,10 +4078,10 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V33" s="48"/>
-      <c r="W33" s="49"/>
-      <c r="X33" s="42"/>
-      <c r="Y33" s="43"/>
+      <c r="V33" s="42"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="48"/>
+      <c r="Y33" s="49"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
@@ -4133,14 +4133,14 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V34" s="44" t="s">
+      <c r="V34" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="W34" s="45"/>
-      <c r="X34" s="38" t="s">
+      <c r="W34" s="39"/>
+      <c r="X34" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="Y34" s="39"/>
+      <c r="Y34" s="45"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
@@ -4192,10 +4192,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V35" s="46"/>
-      <c r="W35" s="47"/>
-      <c r="X35" s="40"/>
-      <c r="Y35" s="41"/>
+      <c r="V35" s="40"/>
+      <c r="W35" s="41"/>
+      <c r="X35" s="46"/>
+      <c r="Y35" s="47"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
@@ -4247,10 +4247,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V36" s="48"/>
-      <c r="W36" s="49"/>
-      <c r="X36" s="42"/>
-      <c r="Y36" s="43"/>
+      <c r="V36" s="42"/>
+      <c r="W36" s="43"/>
+      <c r="X36" s="48"/>
+      <c r="Y36" s="49"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -6216,6 +6216,11 @@
     <sortCondition descending="1" ref="A41:A46"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="X22:Y24"/>
+    <mergeCell ref="V25:W27"/>
+    <mergeCell ref="X25:Y27"/>
+    <mergeCell ref="V28:W30"/>
+    <mergeCell ref="X28:Y30"/>
     <mergeCell ref="V34:W36"/>
     <mergeCell ref="X34:Y36"/>
     <mergeCell ref="T13:T15"/>
@@ -6232,11 +6237,6 @@
     <mergeCell ref="V31:W33"/>
     <mergeCell ref="X31:Y33"/>
     <mergeCell ref="V22:W24"/>
-    <mergeCell ref="X22:Y24"/>
-    <mergeCell ref="V25:W27"/>
-    <mergeCell ref="X25:Y27"/>
-    <mergeCell ref="V28:W30"/>
-    <mergeCell ref="X28:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7968,8 +7968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDBEAB1-8D74-44E1-B064-2F1BCE93660D}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8025,10 +8025,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="20">
-        <v>-215.7</v>
+        <v>-192</v>
       </c>
       <c r="F2" s="20">
-        <v>4.0999999999999996</v>
+        <v>3.4</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>7</v>
@@ -8231,7 +8231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1D9863-0B75-4A54-BECC-533A542694F0}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed example IRMS data filename.
</commit_message>
<xml_diff>
--- a/GCIRMS_Processor/GCIRMS Template.xlsx
+++ b/GCIRMS_Processor/GCIRMS Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881E2B33-43BB-4743-963F-CAE873971BAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E94214-DE63-4C75-A58E-409474132EC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Standards!$A$1:$G$38</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1636,6 +1636,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1652,24 +1670,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3065,14 +3065,14 @@
         <v>126</v>
       </c>
       <c r="U16" s="10"/>
-      <c r="V16" s="38" t="s">
+      <c r="V16" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="W16" s="39"/>
-      <c r="X16" s="44" t="s">
+      <c r="W16" s="45"/>
+      <c r="X16" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="Y16" s="45"/>
+      <c r="Y16" s="39"/>
       <c r="Z16" s="11"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -3128,10 +3128,10 @@
       <c r="S17" s="9"/>
       <c r="T17" s="51"/>
       <c r="U17" s="10"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="46"/>
-      <c r="Y17" s="47"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="40"/>
+      <c r="Y17" s="41"/>
       <c r="Z17" s="11"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -3187,10 +3187,10 @@
       <c r="S18" s="9"/>
       <c r="T18" s="52"/>
       <c r="U18" s="10"/>
-      <c r="V18" s="42"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="48"/>
-      <c r="Y18" s="49"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="43"/>
       <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3248,14 +3248,14 @@
         <v>127</v>
       </c>
       <c r="U19" s="10"/>
-      <c r="V19" s="38" t="s">
+      <c r="V19" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="W19" s="39"/>
-      <c r="X19" s="44" t="s">
+      <c r="W19" s="45"/>
+      <c r="X19" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="Y19" s="45"/>
+      <c r="Y19" s="39"/>
       <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -3311,10 +3311,10 @@
       <c r="S20" s="9"/>
       <c r="T20" s="51"/>
       <c r="U20" s="10"/>
-      <c r="V20" s="40"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="46"/>
-      <c r="Y20" s="47"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="47"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="41"/>
       <c r="Z20" s="11"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -3370,10 +3370,10 @@
       <c r="S21" s="9"/>
       <c r="T21" s="52"/>
       <c r="U21" s="10"/>
-      <c r="V21" s="42"/>
-      <c r="W21" s="43"/>
-      <c r="X21" s="48"/>
-      <c r="Y21" s="49"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="49"/>
+      <c r="X21" s="42"/>
+      <c r="Y21" s="43"/>
       <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3430,14 +3430,14 @@
         <v>135</v>
       </c>
       <c r="U22" s="9"/>
-      <c r="V22" s="38" t="s">
+      <c r="V22" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="W22" s="39"/>
-      <c r="X22" s="44" t="s">
+      <c r="W22" s="45"/>
+      <c r="X22" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="Y22" s="45"/>
+      <c r="Y22" s="39"/>
       <c r="Z22" s="11"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -3492,10 +3492,10 @@
       </c>
       <c r="T23" s="51"/>
       <c r="U23" s="9"/>
-      <c r="V23" s="40"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="46"/>
-      <c r="Y23" s="47"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="47"/>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="41"/>
       <c r="Z23" s="11"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -3550,10 +3550,10 @@
       </c>
       <c r="T24" s="52"/>
       <c r="U24" s="9"/>
-      <c r="V24" s="42"/>
-      <c r="W24" s="43"/>
-      <c r="X24" s="48"/>
-      <c r="Y24" s="49"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="49"/>
+      <c r="X24" s="42"/>
+      <c r="Y24" s="43"/>
       <c r="Z24" s="11"/>
     </row>
     <row r="25" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3610,14 +3610,14 @@
         <v>129</v>
       </c>
       <c r="U25" s="9"/>
-      <c r="V25" s="38" t="s">
+      <c r="V25" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="W25" s="39"/>
-      <c r="X25" s="44" t="s">
+      <c r="W25" s="45"/>
+      <c r="X25" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="Y25" s="45"/>
+      <c r="Y25" s="39"/>
       <c r="Z25" s="11"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3672,10 +3672,10 @@
       </c>
       <c r="T26" s="54"/>
       <c r="U26" s="9"/>
-      <c r="V26" s="40"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="46"/>
-      <c r="Y26" s="47"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="40"/>
+      <c r="Y26" s="41"/>
       <c r="Z26" s="11"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -3730,10 +3730,10 @@
       </c>
       <c r="T27" s="54"/>
       <c r="U27" s="9"/>
-      <c r="V27" s="42"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="48"/>
-      <c r="Y27" s="49"/>
+      <c r="V27" s="48"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="42"/>
+      <c r="Y27" s="43"/>
       <c r="Z27" s="11"/>
     </row>
     <row r="28" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3788,14 +3788,14 @@
       </c>
       <c r="T28" s="54"/>
       <c r="U28" s="9"/>
-      <c r="V28" s="38" t="s">
+      <c r="V28" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="W28" s="39"/>
-      <c r="X28" s="44" t="s">
+      <c r="W28" s="45"/>
+      <c r="X28" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="Y28" s="45"/>
+      <c r="Y28" s="39"/>
       <c r="Z28" s="11"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -3850,10 +3850,10 @@
       </c>
       <c r="T29" s="54"/>
       <c r="U29" s="9"/>
-      <c r="V29" s="40"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="46"/>
-      <c r="Y29" s="47"/>
+      <c r="V29" s="46"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="41"/>
       <c r="Z29" s="11"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -3908,10 +3908,10 @@
       </c>
       <c r="T30" s="55"/>
       <c r="U30" s="9"/>
-      <c r="V30" s="42"/>
-      <c r="W30" s="43"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="49"/>
+      <c r="V30" s="48"/>
+      <c r="W30" s="49"/>
+      <c r="X30" s="42"/>
+      <c r="Y30" s="43"/>
       <c r="Z30" s="11"/>
     </row>
     <row r="31" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3964,14 +3964,14 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V31" s="38" t="s">
+      <c r="V31" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="W31" s="39"/>
-      <c r="X31" s="44" t="s">
+      <c r="W31" s="45"/>
+      <c r="X31" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="Y31" s="45"/>
+      <c r="Y31" s="39"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
@@ -4023,10 +4023,10 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V32" s="40"/>
-      <c r="W32" s="41"/>
-      <c r="X32" s="46"/>
-      <c r="Y32" s="47"/>
+      <c r="V32" s="46"/>
+      <c r="W32" s="47"/>
+      <c r="X32" s="40"/>
+      <c r="Y32" s="41"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
@@ -4078,10 +4078,10 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V33" s="42"/>
-      <c r="W33" s="43"/>
-      <c r="X33" s="48"/>
-      <c r="Y33" s="49"/>
+      <c r="V33" s="48"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="43"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
@@ -4133,14 +4133,14 @@
         <f t="shared" si="2"/>
         <v>14.82</v>
       </c>
-      <c r="V34" s="38" t="s">
+      <c r="V34" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="W34" s="39"/>
-      <c r="X34" s="44" t="s">
+      <c r="W34" s="45"/>
+      <c r="X34" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="Y34" s="45"/>
+      <c r="Y34" s="39"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
@@ -4192,10 +4192,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V35" s="40"/>
-      <c r="W35" s="41"/>
-      <c r="X35" s="46"/>
-      <c r="Y35" s="47"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="47"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="41"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
@@ -4247,10 +4247,10 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="V36" s="42"/>
-      <c r="W36" s="43"/>
-      <c r="X36" s="48"/>
-      <c r="Y36" s="49"/>
+      <c r="V36" s="48"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="43"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -6216,11 +6216,6 @@
     <sortCondition descending="1" ref="A41:A46"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="X22:Y24"/>
-    <mergeCell ref="V25:W27"/>
-    <mergeCell ref="X25:Y27"/>
-    <mergeCell ref="V28:W30"/>
-    <mergeCell ref="X28:Y30"/>
     <mergeCell ref="V34:W36"/>
     <mergeCell ref="X34:Y36"/>
     <mergeCell ref="T13:T15"/>
@@ -6237,6 +6232,11 @@
     <mergeCell ref="V31:W33"/>
     <mergeCell ref="X31:Y33"/>
     <mergeCell ref="V22:W24"/>
+    <mergeCell ref="X22:Y24"/>
+    <mergeCell ref="V25:W27"/>
+    <mergeCell ref="X25:Y27"/>
+    <mergeCell ref="V28:W30"/>
+    <mergeCell ref="X28:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6249,7 +6249,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7968,7 +7968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDBEAB1-8D74-44E1-B064-2F1BCE93660D}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -8231,7 +8231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1D9863-0B75-4A54-BECC-533A542694F0}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added estimated values for the LCA standard mix.
</commit_message>
<xml_diff>
--- a/GCIRMS_Processor/GCIRMS Template.xlsx
+++ b/GCIRMS_Processor/GCIRMS Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5C317E-E140-421C-AA6A-6D70000DEF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDAB0DE-9937-40D7-AA05-8EFCCE73A536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Initials" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Standards!$A$1:$G$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Standards!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="279">
   <si>
     <t>id1</t>
   </si>
@@ -167,15 +167,6 @@
     <t>control</t>
   </si>
   <si>
-    <t>F8</t>
-  </si>
-  <si>
-    <t>FAEE</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
     <t>C16</t>
   </si>
   <si>
@@ -183,9 +174,6 @@
   </si>
   <si>
     <t>dD_known_sd</t>
-  </si>
-  <si>
-    <t>A7</t>
   </si>
   <si>
     <t>C22</t>
@@ -1189,24 +1177,6 @@
     <t>GC Sleep.met</t>
   </si>
   <si>
-    <t>C20 + C30 FAMEs</t>
-  </si>
-  <si>
-    <t>C20 + C28 FAMEs</t>
-  </si>
-  <si>
-    <t>C4 Mix</t>
-  </si>
-  <si>
-    <t>C18 + C24 FAMEs</t>
-  </si>
-  <si>
-    <t>C27 + C31 Alkanes</t>
-  </si>
-  <si>
-    <t>C22 + C25 + C35 Alkanes</t>
-  </si>
-  <si>
     <t>C35</t>
   </si>
   <si>
@@ -1214,9 +1184,6 @@
   </si>
   <si>
     <t>Type the name (matching your IRMS export Identifier 1 name) of the standard mix to use for scale normalization.</t>
-  </si>
-  <si>
-    <t>Jeff QAQC</t>
   </si>
   <si>
     <t>ACAL</t>
@@ -1614,7 +1581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1659,7 +1626,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1735,6 +1701,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1751,24 +1735,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2123,90 +2089,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B3" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="B4" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="27" t="s">
+      <c r="B5" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C5" s="12" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="27" t="s">
+    <row r="6" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>158</v>
-      </c>
       <c r="C7" s="12" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>187</v>
+      <c r="A8" s="26" t="s">
+        <v>183</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2299,19 +2265,19 @@
         <v>39</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>32</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -2344,13 +2310,13 @@
         <v>1</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5">
@@ -2365,10 +2331,10 @@
         <v>46.7</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="U2" s="6" t="str">
         <f>INDEX(U7:U8,MATCH(T10,T7:T8,0))</f>
@@ -2408,13 +2374,13 @@
         <v>1</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5">
@@ -2429,13 +2395,13 @@
         <v>46.7</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="V3" s="6">
         <v>46.7</v>
@@ -2471,13 +2437,13 @@
         <v>1</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5">
@@ -2492,13 +2458,13 @@
         <v>46.7</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="V4" s="6">
         <f>V2-43.93</f>
@@ -2535,13 +2501,13 @@
         <v>1</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5">
@@ -2586,16 +2552,16 @@
         <v>3</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K6" s="5" t="str">
         <f>Samples!$A$2</f>
         <v>CA02</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M6" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="M6" s="41"/>
       <c r="N6" s="5">
         <v>20</v>
       </c>
@@ -2608,13 +2574,13 @@
         <v>56.75</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -2647,16 +2613,16 @@
         <v>3</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K7" s="5" t="str">
         <f>Samples!$A$2</f>
         <v>CA02</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M7" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="M7" s="41"/>
       <c r="N7" s="5">
         <v>20</v>
       </c>
@@ -2673,10 +2639,10 @@
         <v>44.709999999999994</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2709,16 +2675,16 @@
         <v>4</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K8" s="5" t="str">
         <f>Samples!$A$3</f>
         <v>CA10</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M8" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="M8" s="41"/>
       <c r="N8" s="5">
         <v>20</v>
       </c>
@@ -2731,11 +2697,11 @@
         <v>56.75</v>
       </c>
       <c r="S8" s="7"/>
-      <c r="T8" s="38" t="s">
-        <v>251</v>
+      <c r="T8" s="37" t="s">
+        <v>247</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -2768,16 +2734,16 @@
         <v>4</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K9" s="5" t="str">
         <f>Samples!$A$3</f>
         <v>CA10</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M9" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="M9" s="41"/>
       <c r="N9" s="5">
         <v>20</v>
       </c>
@@ -2790,8 +2756,8 @@
         <v>56.75</v>
       </c>
       <c r="S9" s="9"/>
-      <c r="T9" s="40" t="s">
-        <v>254</v>
+      <c r="T9" s="39" t="s">
+        <v>250</v>
       </c>
       <c r="U9" s="11"/>
     </row>
@@ -2825,16 +2791,16 @@
         <v>5</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K10" s="5" t="str">
         <f>Samples!$A$4</f>
         <v>CA14</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M10" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="M10" s="41"/>
       <c r="N10" s="5">
         <v>20</v>
       </c>
@@ -2847,8 +2813,8 @@
         <v>56.75</v>
       </c>
       <c r="S10" s="9"/>
-      <c r="T10" s="39" t="s">
-        <v>250</v>
+      <c r="T10" s="38" t="s">
+        <v>246</v>
       </c>
       <c r="U10" s="11"/>
     </row>
@@ -2882,16 +2848,16 @@
         <v>5</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K11" s="5" t="str">
         <f>Samples!$A$4</f>
         <v>CA14</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M11" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="M11" s="41"/>
       <c r="N11" s="5">
         <v>20</v>
       </c>
@@ -2903,7 +2869,7 @@
         <f t="shared" si="2"/>
         <v>56.75</v>
       </c>
-      <c r="T11" s="37"/>
+      <c r="T11" s="36"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
@@ -2935,14 +2901,14 @@
         <v>6</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K12" s="5" t="str">
         <f>Samples!$A$5</f>
         <v>CA18</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5">
@@ -2992,14 +2958,14 @@
         <v>6</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K13" s="5" t="str">
         <f>Samples!$A$5</f>
         <v>CA18</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5">
@@ -3014,18 +2980,18 @@
         <v>56.75</v>
       </c>
       <c r="S13" s="9"/>
-      <c r="T13" s="57" t="s">
-        <v>118</v>
+      <c r="T13" s="56" t="s">
+        <v>114</v>
       </c>
       <c r="U13" s="10"/>
-      <c r="V13" s="63" t="s">
-        <v>116</v>
-      </c>
-      <c r="W13" s="64"/>
-      <c r="X13" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y13" s="70"/>
+      <c r="V13" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="W13" s="63"/>
+      <c r="X13" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y13" s="69"/>
       <c r="Z13" s="11"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -3058,13 +3024,13 @@
         <v>1</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="5">
@@ -3079,12 +3045,12 @@
         <v>46.7</v>
       </c>
       <c r="S14" s="9"/>
-      <c r="T14" s="58"/>
+      <c r="T14" s="57"/>
       <c r="U14" s="10"/>
-      <c r="V14" s="65"/>
-      <c r="W14" s="66"/>
-      <c r="X14" s="71"/>
-      <c r="Y14" s="72"/>
+      <c r="V14" s="64"/>
+      <c r="W14" s="65"/>
+      <c r="X14" s="70"/>
+      <c r="Y14" s="71"/>
       <c r="Z14" s="11"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -3117,13 +3083,13 @@
         <v>1</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5">
@@ -3138,12 +3104,12 @@
         <v>46.7</v>
       </c>
       <c r="S15" s="9"/>
-      <c r="T15" s="59"/>
+      <c r="T15" s="58"/>
       <c r="U15" s="10"/>
-      <c r="V15" s="67"/>
-      <c r="W15" s="68"/>
-      <c r="X15" s="73"/>
-      <c r="Y15" s="74"/>
+      <c r="V15" s="66"/>
+      <c r="W15" s="67"/>
+      <c r="X15" s="72"/>
+      <c r="Y15" s="73"/>
       <c r="Z15" s="11"/>
     </row>
     <row r="16" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3176,16 +3142,16 @@
         <v>19</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42">
+      <c r="M16" s="41"/>
+      <c r="N16" s="41">
         <v>30</v>
       </c>
       <c r="O16" s="5" t="str">
@@ -3197,18 +3163,18 @@
         <v>46.7</v>
       </c>
       <c r="S16" s="9"/>
-      <c r="T16" s="57" t="s">
-        <v>112</v>
+      <c r="T16" s="56" t="s">
+        <v>108</v>
       </c>
       <c r="U16" s="10"/>
-      <c r="V16" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="W16" s="52"/>
-      <c r="X16" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y16" s="46"/>
+      <c r="V16" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="W16" s="45"/>
+      <c r="X16" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y16" s="51"/>
       <c r="Z16" s="11"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -3241,16 +3207,16 @@
         <v>20</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42">
+      <c r="M17" s="41"/>
+      <c r="N17" s="41">
         <v>25</v>
       </c>
       <c r="O17" s="5" t="str">
@@ -3262,12 +3228,12 @@
         <v>46.7</v>
       </c>
       <c r="S17" s="9"/>
-      <c r="T17" s="58"/>
+      <c r="T17" s="57"/>
       <c r="U17" s="10"/>
-      <c r="V17" s="53"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="48"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="52"/>
+      <c r="Y17" s="53"/>
       <c r="Z17" s="11"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -3300,16 +3266,16 @@
         <v>21</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42">
+      <c r="M18" s="41"/>
+      <c r="N18" s="41">
         <v>20</v>
       </c>
       <c r="O18" s="5" t="str">
@@ -3321,12 +3287,12 @@
         <v>46.7</v>
       </c>
       <c r="S18" s="9"/>
-      <c r="T18" s="59"/>
+      <c r="T18" s="58"/>
       <c r="U18" s="10"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="56"/>
-      <c r="X18" s="49"/>
-      <c r="Y18" s="50"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="54"/>
+      <c r="Y18" s="55"/>
       <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3359,16 +3325,16 @@
         <v>22</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42">
+      <c r="M19" s="41"/>
+      <c r="N19" s="41">
         <v>15</v>
       </c>
       <c r="O19" s="5" t="str">
@@ -3380,18 +3346,18 @@
         <v>46.7</v>
       </c>
       <c r="S19" s="9"/>
-      <c r="T19" s="57" t="s">
-        <v>113</v>
+      <c r="T19" s="56" t="s">
+        <v>109</v>
       </c>
       <c r="U19" s="10"/>
-      <c r="V19" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="W19" s="52"/>
-      <c r="X19" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y19" s="46"/>
+      <c r="V19" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="W19" s="45"/>
+      <c r="X19" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y19" s="51"/>
       <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -3424,16 +3390,16 @@
         <v>23</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42">
+      <c r="M20" s="41"/>
+      <c r="N20" s="41">
         <v>10</v>
       </c>
       <c r="O20" s="5" t="str">
@@ -3445,12 +3411,12 @@
         <v>46.7</v>
       </c>
       <c r="S20" s="9"/>
-      <c r="T20" s="58"/>
+      <c r="T20" s="57"/>
       <c r="U20" s="10"/>
-      <c r="V20" s="53"/>
-      <c r="W20" s="54"/>
-      <c r="X20" s="47"/>
-      <c r="Y20" s="48"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="47"/>
+      <c r="X20" s="52"/>
+      <c r="Y20" s="53"/>
       <c r="Z20" s="11"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -3483,16 +3449,16 @@
         <v>24</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42">
+      <c r="M21" s="41"/>
+      <c r="N21" s="41">
         <v>5</v>
       </c>
       <c r="O21" s="5" t="str">
@@ -3504,12 +3470,12 @@
         <v>46.7</v>
       </c>
       <c r="S21" s="9"/>
-      <c r="T21" s="59"/>
+      <c r="T21" s="58"/>
       <c r="U21" s="10"/>
-      <c r="V21" s="55"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="49"/>
-      <c r="Y21" s="50"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="49"/>
+      <c r="X21" s="54"/>
+      <c r="Y21" s="55"/>
       <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3542,7 +3508,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>9</v>
@@ -3562,18 +3528,18 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T22" s="57" t="s">
-        <v>121</v>
+      <c r="T22" s="56" t="s">
+        <v>117</v>
       </c>
       <c r="U22" s="9"/>
-      <c r="V22" s="51" t="s">
+      <c r="V22" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="W22" s="52"/>
-      <c r="X22" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y22" s="46"/>
+      <c r="W22" s="45"/>
+      <c r="X22" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y22" s="51"/>
       <c r="Z22" s="11"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -3606,7 +3572,7 @@
         <v>2</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>9</v>
@@ -3626,12 +3592,12 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T23" s="58"/>
+      <c r="T23" s="57"/>
       <c r="U23" s="9"/>
-      <c r="V23" s="53"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="47"/>
-      <c r="Y23" s="48"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="47"/>
+      <c r="X23" s="52"/>
+      <c r="Y23" s="53"/>
       <c r="Z23" s="11"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -3664,13 +3630,13 @@
         <v>1</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5">
@@ -3684,12 +3650,12 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T24" s="59"/>
+      <c r="T24" s="58"/>
       <c r="U24" s="9"/>
-      <c r="V24" s="55"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="49"/>
-      <c r="Y24" s="50"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="49"/>
+      <c r="X24" s="54"/>
+      <c r="Y24" s="55"/>
       <c r="Z24" s="11"/>
     </row>
     <row r="25" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3722,13 +3688,13 @@
         <v>1</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5">
@@ -3742,18 +3708,18 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T25" s="60" t="s">
-        <v>115</v>
+      <c r="T25" s="59" t="s">
+        <v>111</v>
       </c>
       <c r="U25" s="9"/>
-      <c r="V25" s="51" t="s">
-        <v>122</v>
-      </c>
-      <c r="W25" s="52"/>
-      <c r="X25" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y25" s="46"/>
+      <c r="V25" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="W25" s="45"/>
+      <c r="X25" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y25" s="51"/>
       <c r="Z25" s="11"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3786,7 +3752,7 @@
         <v>7</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K26" s="5" t="str">
         <f>Samples!$A$6</f>
@@ -3807,12 +3773,12 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T26" s="61"/>
+      <c r="T26" s="60"/>
       <c r="U26" s="9"/>
-      <c r="V26" s="53"/>
-      <c r="W26" s="54"/>
-      <c r="X26" s="47"/>
-      <c r="Y26" s="48"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="52"/>
+      <c r="Y26" s="53"/>
       <c r="Z26" s="11"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -3845,7 +3811,7 @@
         <v>7</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K27" s="5" t="str">
         <f>Samples!$A$6</f>
@@ -3866,12 +3832,12 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T27" s="61"/>
+      <c r="T27" s="60"/>
       <c r="U27" s="9"/>
-      <c r="V27" s="55"/>
-      <c r="W27" s="56"/>
-      <c r="X27" s="49"/>
-      <c r="Y27" s="50"/>
+      <c r="V27" s="48"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="54"/>
+      <c r="Y27" s="55"/>
       <c r="Z27" s="11"/>
     </row>
     <row r="28" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3904,7 +3870,7 @@
         <v>8</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K28" s="5" t="str">
         <f>Samples!$A$7</f>
@@ -3925,16 +3891,16 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T28" s="61"/>
+      <c r="T28" s="60"/>
       <c r="U28" s="9"/>
-      <c r="V28" s="51" t="s">
+      <c r="V28" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="W28" s="52"/>
-      <c r="X28" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y28" s="46"/>
+      <c r="W28" s="45"/>
+      <c r="X28" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y28" s="51"/>
       <c r="Z28" s="11"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -3967,7 +3933,7 @@
         <v>8</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K29" s="5" t="str">
         <f>Samples!$A$7</f>
@@ -3988,12 +3954,12 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T29" s="61"/>
+      <c r="T29" s="60"/>
       <c r="U29" s="9"/>
-      <c r="V29" s="53"/>
-      <c r="W29" s="54"/>
-      <c r="X29" s="47"/>
-      <c r="Y29" s="48"/>
+      <c r="V29" s="46"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="52"/>
+      <c r="Y29" s="53"/>
       <c r="Z29" s="11"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -4026,14 +3992,14 @@
         <v>9</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K30" s="5" t="str">
         <f>Samples!$A$8</f>
         <v>BOF1-11</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M30" s="5"/>
       <c r="N30" s="5">
@@ -4047,12 +4013,12 @@
         <f t="shared" si="2"/>
         <v>56.75</v>
       </c>
-      <c r="T30" s="62"/>
+      <c r="T30" s="61"/>
       <c r="U30" s="9"/>
-      <c r="V30" s="55"/>
-      <c r="W30" s="56"/>
-      <c r="X30" s="49"/>
-      <c r="Y30" s="50"/>
+      <c r="V30" s="48"/>
+      <c r="W30" s="49"/>
+      <c r="X30" s="54"/>
+      <c r="Y30" s="55"/>
       <c r="Z30" s="11"/>
     </row>
     <row r="31" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4085,14 +4051,14 @@
         <v>9</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K31" s="5" t="str">
         <f>Samples!$A$8</f>
         <v>BOF1-11</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M31" s="5"/>
       <c r="N31" s="5">
@@ -4106,14 +4072,14 @@
         <f t="shared" si="2"/>
         <v>56.75</v>
       </c>
-      <c r="V31" s="51" t="s">
-        <v>203</v>
-      </c>
-      <c r="W31" s="52"/>
-      <c r="X31" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="Y31" s="46"/>
+      <c r="V31" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="W31" s="45"/>
+      <c r="X31" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y31" s="51"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
@@ -4145,14 +4111,14 @@
         <v>10</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K32" s="5" t="str">
         <f>Samples!$A$9</f>
         <v>BOF1-31</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M32" s="5"/>
       <c r="N32" s="5">
@@ -4166,10 +4132,10 @@
         <f t="shared" si="2"/>
         <v>56.75</v>
       </c>
-      <c r="V32" s="53"/>
-      <c r="W32" s="54"/>
-      <c r="X32" s="47"/>
-      <c r="Y32" s="48"/>
+      <c r="V32" s="46"/>
+      <c r="W32" s="47"/>
+      <c r="X32" s="52"/>
+      <c r="Y32" s="53"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
@@ -4201,14 +4167,14 @@
         <v>10</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K33" s="5" t="str">
         <f>Samples!$A$9</f>
         <v>BOF1-31</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M33" s="5"/>
       <c r="N33" s="5">
@@ -4222,10 +4188,10 @@
         <f t="shared" si="2"/>
         <v>56.75</v>
       </c>
-      <c r="V33" s="55"/>
-      <c r="W33" s="56"/>
-      <c r="X33" s="49"/>
-      <c r="Y33" s="50"/>
+      <c r="V33" s="48"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="54"/>
+      <c r="Y33" s="55"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
@@ -4257,13 +4223,13 @@
         <v>1</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M34" s="5"/>
       <c r="N34" s="5">
@@ -4277,14 +4243,14 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="V34" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="W34" s="52"/>
-      <c r="X34" s="45" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y34" s="46"/>
+      <c r="V34" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="W34" s="45"/>
+      <c r="X34" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y34" s="51"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
@@ -4316,13 +4282,13 @@
         <v>1</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M35" s="5"/>
       <c r="N35" s="5">
@@ -4336,10 +4302,10 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="V35" s="53"/>
-      <c r="W35" s="54"/>
-      <c r="X35" s="47"/>
-      <c r="Y35" s="48"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="47"/>
+      <c r="X35" s="52"/>
+      <c r="Y35" s="53"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
@@ -4371,7 +4337,7 @@
         <v>2</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>9</v>
@@ -4391,10 +4357,10 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="V36" s="55"/>
-      <c r="W36" s="56"/>
-      <c r="X36" s="49"/>
-      <c r="Y36" s="50"/>
+      <c r="V36" s="48"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="54"/>
+      <c r="Y36" s="55"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -4426,7 +4392,7 @@
         <v>2</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>9</v>
@@ -4477,16 +4443,16 @@
         <v>19</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M38" s="42"/>
-      <c r="N38" s="42">
+      <c r="M38" s="41"/>
+      <c r="N38" s="41">
         <v>30</v>
       </c>
       <c r="O38" s="5" t="str">
@@ -4528,16 +4494,16 @@
         <v>20</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M39" s="42"/>
-      <c r="N39" s="42">
+      <c r="M39" s="41"/>
+      <c r="N39" s="41">
         <v>25</v>
       </c>
       <c r="O39" s="5" t="str">
@@ -4579,16 +4545,16 @@
         <v>21</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M40" s="42"/>
-      <c r="N40" s="42">
+      <c r="M40" s="41"/>
+      <c r="N40" s="41">
         <v>20</v>
       </c>
       <c r="O40" s="5" t="str">
@@ -4630,16 +4596,16 @@
         <v>22</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M41" s="42"/>
-      <c r="N41" s="42">
+      <c r="M41" s="41"/>
+      <c r="N41" s="41">
         <v>15</v>
       </c>
       <c r="O41" s="5" t="str">
@@ -4681,16 +4647,16 @@
         <v>23</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M42" s="42"/>
-      <c r="N42" s="42">
+      <c r="M42" s="41"/>
+      <c r="N42" s="41">
         <v>10</v>
       </c>
       <c r="O42" s="5" t="str">
@@ -4732,16 +4698,16 @@
         <v>24</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M43" s="42"/>
-      <c r="N43" s="42">
+      <c r="M43" s="41"/>
+      <c r="N43" s="41">
         <v>5</v>
       </c>
       <c r="O43" s="5" t="str">
@@ -4783,13 +4749,13 @@
         <v>1</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="5">
@@ -4834,13 +4800,13 @@
         <v>1</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M45" s="5"/>
       <c r="N45" s="5">
@@ -4885,7 +4851,7 @@
         <v>11</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K46" s="5" t="str">
         <f>Samples!$A$10</f>
@@ -4937,7 +4903,7 @@
         <v>11</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K47" s="5" t="str">
         <f>Samples!$A$10</f>
@@ -4989,7 +4955,7 @@
         <v>12</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K48" s="5" t="str">
         <f>Samples!$A$11</f>
@@ -5041,7 +5007,7 @@
         <v>12</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K49" s="5" t="str">
         <f>Samples!$A$11</f>
@@ -5093,14 +5059,14 @@
         <v>13</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>Samples!$A$12</f>
         <v>BOF1-41</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M50" s="5"/>
       <c r="N50" s="5">
@@ -5145,14 +5111,14 @@
         <v>13</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K51" s="5" t="str">
         <f>Samples!$A$12</f>
         <v>BOF1-41</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M51" s="5"/>
       <c r="N51" s="5">
@@ -5197,14 +5163,14 @@
         <v>14</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K52" s="5" t="str">
         <f>Samples!$A$13</f>
         <v>NE 0-5 cm</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M52" s="5"/>
       <c r="N52" s="5">
@@ -5249,14 +5215,14 @@
         <v>14</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K53" s="5" t="str">
         <f>Samples!$A$13</f>
         <v>NE 0-5 cm</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M53" s="5"/>
       <c r="N53" s="5">
@@ -5301,13 +5267,13 @@
         <v>1</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M54" s="5"/>
       <c r="N54" s="5">
@@ -5352,13 +5318,13 @@
         <v>1</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M55" s="5"/>
       <c r="N55" s="5">
@@ -5396,20 +5362,20 @@
         <v>24</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I56" s="5">
         <v>54</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
       <c r="O56" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
@@ -5850,6 +5816,11 @@
     <sortCondition descending="1" ref="A41:A46"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="X22:Y24"/>
+    <mergeCell ref="V25:W27"/>
+    <mergeCell ref="X25:Y27"/>
+    <mergeCell ref="V28:W30"/>
+    <mergeCell ref="X28:Y30"/>
     <mergeCell ref="V34:W36"/>
     <mergeCell ref="X34:Y36"/>
     <mergeCell ref="T13:T15"/>
@@ -5866,11 +5837,6 @@
     <mergeCell ref="V31:W33"/>
     <mergeCell ref="X31:Y33"/>
     <mergeCell ref="V22:W24"/>
-    <mergeCell ref="X22:Y24"/>
-    <mergeCell ref="V25:W27"/>
-    <mergeCell ref="X25:Y27"/>
-    <mergeCell ref="V28:W30"/>
-    <mergeCell ref="X28:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -5923,161 +5889,161 @@
         <v>3</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>210</v>
+        <v>57</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>206</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26">
+        <v>263</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25">
         <f>G2/20</f>
         <v>1350</v>
       </c>
-      <c r="G2" s="43">
+      <c r="G2" s="42">
         <f>27000</f>
         <v>27000</v>
       </c>
-      <c r="H2" s="58"/>
+      <c r="H2" s="57"/>
       <c r="I2" s="16" t="s">
         <v>35</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26">
+        <v>264</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25">
         <f t="shared" ref="F3:F13" si="0">G3/20</f>
         <v>347.7</v>
       </c>
-      <c r="G3" s="44">
+      <c r="G3" s="43">
         <v>6954</v>
       </c>
-      <c r="H3" s="58"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="16" t="s">
         <v>22</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26">
+        <v>265</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25">
         <f t="shared" si="0"/>
         <v>202.3</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="43">
         <v>4046</v>
       </c>
-      <c r="H4" s="58"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="16" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26">
+        <v>266</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25">
         <f t="shared" si="0"/>
         <v>86.35</v>
       </c>
-      <c r="G5" s="44">
+      <c r="G5" s="43">
         <v>1727</v>
       </c>
-      <c r="H5" s="58"/>
+      <c r="H5" s="57"/>
       <c r="I5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="58"/>
+        <v>258</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="57"/>
       <c r="I6" s="16" t="s">
         <v>3</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="58"/>
+        <v>258</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="57"/>
       <c r="I7" s="16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="F8" s="26">
+        <v>267</v>
+      </c>
+      <c r="F8" s="25">
         <f t="shared" si="0"/>
         <v>373.15</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="43">
         <v>7463</v>
       </c>
-      <c r="H8" s="59"/>
+      <c r="H8" s="58"/>
       <c r="I8" s="16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26">
+        <v>268</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25">
         <f t="shared" si="0"/>
         <v>399.3</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="43">
         <v>7986</v>
       </c>
       <c r="H9" s="15"/>
@@ -6086,42 +6052,42 @@
       <c r="A10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="44"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26">
+        <v>269</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25">
         <f>G12/20</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="G12" s="43">
+      <c r="G12" s="42">
         <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26">
+        <v>270</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25">
         <f t="shared" si="0"/>
         <v>397.71625081846406</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="43">
         <v>7954.325016369281</v>
       </c>
     </row>
@@ -6140,10 +6106,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6171,30 +6137,30 @@
         <v>11</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="75" t="s">
-        <v>127</v>
+        <v>48</v>
+      </c>
+      <c r="H1" s="74" t="s">
+        <v>123</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>13</v>
@@ -6214,17 +6180,17 @@
       <c r="G2" s="15">
         <v>118</v>
       </c>
-      <c r="H2" s="75"/>
+      <c r="H2" s="74"/>
       <c r="I2" s="16" t="s">
         <v>35</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>5</v>
@@ -6244,17 +6210,17 @@
       <c r="G3" s="15">
         <v>5</v>
       </c>
-      <c r="H3" s="75"/>
+      <c r="H3" s="74"/>
       <c r="I3" s="16" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>19</v>
@@ -6274,22 +6240,22 @@
       <c r="G4" s="15">
         <v>5</v>
       </c>
-      <c r="H4" s="75" t="s">
-        <v>128</v>
+      <c r="H4" s="74" t="s">
+        <v>124</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>12</v>
@@ -6306,12 +6272,12 @@
       <c r="G5" s="15">
         <v>9</v>
       </c>
-      <c r="H5" s="75"/>
+      <c r="H5" s="74"/>
       <c r="I5" s="16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -6336,12 +6302,12 @@
       <c r="G6" s="15">
         <v>7</v>
       </c>
-      <c r="H6" s="75"/>
+      <c r="H6" s="74"/>
       <c r="I6" s="16" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -6367,10 +6333,10 @@
         <v>5</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -6396,10 +6362,10 @@
         <v>6</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -6535,194 +6501,164 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>42</v>
+        <v>201</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>44</v>
+        <v>203</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>4</v>
+        <v>202</v>
       </c>
       <c r="D16" s="14">
         <v>1</v>
       </c>
       <c r="E16" s="15">
-        <v>-231.2</v>
+        <v>-81.900000000000006</v>
       </c>
       <c r="F16" s="15">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="G16" s="15">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>42</v>
+        <v>258</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="D17" s="14">
         <v>1</v>
       </c>
-      <c r="E17" s="15">
-        <v>-231.2</v>
-      </c>
-      <c r="F17" s="15">
-        <v>2.7</v>
-      </c>
-      <c r="G17" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="40">
+        <v>-67.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>42</v>
+        <v>258</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D18" s="14">
         <v>1</v>
       </c>
-      <c r="E18" s="15">
-        <v>-166.8</v>
-      </c>
-      <c r="F18" s="15">
-        <v>1.7</v>
-      </c>
-      <c r="G18" s="15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="40">
+        <v>-263.60000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>42</v>
+        <v>258</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="D19" s="14">
         <v>1</v>
       </c>
-      <c r="E19" s="15">
-        <v>-211</v>
-      </c>
-      <c r="F19" s="15">
-        <v>1.7</v>
-      </c>
-      <c r="G19" s="15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="40">
+        <v>-172.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>42</v>
+        <v>258</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D20" s="14">
         <v>1</v>
       </c>
-      <c r="E20" s="15">
-        <v>-206.2</v>
-      </c>
-      <c r="F20" s="15">
-        <v>1.7</v>
-      </c>
-      <c r="G20" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="40">
+        <v>-85.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>42</v>
+        <v>258</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="D21" s="14">
         <v>1</v>
       </c>
-      <c r="E21" s="15">
-        <v>-214.2</v>
-      </c>
-      <c r="F21" s="15">
-        <v>0.7</v>
-      </c>
-      <c r="G21" s="15">
-        <v>4</v>
+      <c r="E21" s="40">
+        <v>-271.89999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>42</v>
+        <v>259</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D22" s="14">
         <v>1</v>
       </c>
       <c r="E22" s="15">
-        <v>-166.7</v>
+        <v>-167.2</v>
       </c>
       <c r="F22" s="15">
         <v>0.3</v>
       </c>
       <c r="G22" s="15">
-        <v>3</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>42</v>
+        <v>259</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="D23" s="14">
         <v>1</v>
       </c>
       <c r="E23" s="15">
-        <v>-195.5</v>
+        <v>-67.599999999999994</v>
       </c>
       <c r="F23" s="15">
-        <v>1.2</v>
+        <v>0.3</v>
       </c>
       <c r="G23" s="15">
-        <v>4</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>48</v>
+        <v>259</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>12</v>
@@ -6730,22 +6666,22 @@
       <c r="D24" s="14">
         <v>1</v>
       </c>
-      <c r="E24" s="18">
-        <v>-9.1</v>
+      <c r="E24" s="15">
+        <v>-203.5</v>
       </c>
       <c r="F24" s="15">
-        <v>1.4</v>
+        <v>0.3</v>
       </c>
       <c r="G24" s="15">
-        <v>7</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>48</v>
+        <v>259</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>12</v>
@@ -6754,21 +6690,21 @@
         <v>1</v>
       </c>
       <c r="E25" s="15">
-        <v>-117.5</v>
+        <v>-204.8</v>
       </c>
       <c r="F25" s="15">
-        <v>2.1</v>
+        <v>0.3</v>
       </c>
       <c r="G25" s="15">
-        <v>8</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>48</v>
+        <v>259</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>12</v>
@@ -6777,21 +6713,21 @@
         <v>1</v>
       </c>
       <c r="E26" s="15">
-        <v>-52</v>
+        <v>-184.9</v>
       </c>
       <c r="F26" s="15">
-        <v>1.1000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="G26" s="15">
-        <v>5</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>48</v>
+        <v>259</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>12</v>
@@ -6800,21 +6736,21 @@
         <v>1</v>
       </c>
       <c r="E27" s="15">
-        <v>-56.3</v>
+        <v>-124.9</v>
       </c>
       <c r="F27" s="15">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="G27" s="15">
-        <v>5</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>48</v>
+        <v>259</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>13</v>
+        <v>271</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>12</v>
@@ -6823,21 +6759,21 @@
         <v>1</v>
       </c>
       <c r="E28" s="15">
-        <v>-177.6</v>
+        <v>-134.19999999999999</v>
       </c>
       <c r="F28" s="15">
-        <v>1.1000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="G28" s="15">
-        <v>5</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>48</v>
+        <v>259</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>16</v>
+        <v>255</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>12</v>
@@ -6846,870 +6782,16 @@
         <v>1</v>
       </c>
       <c r="E29" s="15">
-        <v>-177.8</v>
+        <v>-193.5</v>
       </c>
       <c r="F29" s="15">
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="G29" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="14">
-        <v>1</v>
-      </c>
-      <c r="E30" s="15">
-        <v>-75.8</v>
-      </c>
-      <c r="F30" s="15">
-        <v>1.8</v>
-      </c>
-      <c r="G30" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="14">
-        <v>1</v>
-      </c>
-      <c r="E31" s="15">
-        <v>-67.2</v>
-      </c>
-      <c r="F31" s="15">
-        <v>1</v>
-      </c>
-      <c r="G31" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="14">
-        <v>1</v>
-      </c>
-      <c r="E32" s="15">
-        <v>-29.7</v>
-      </c>
-      <c r="F32" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="G32" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="14">
-        <v>1</v>
-      </c>
-      <c r="E33" s="15">
-        <v>-263.60000000000002</v>
-      </c>
-      <c r="F33" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G33" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="14">
-        <v>1</v>
-      </c>
-      <c r="E34" s="15">
-        <v>-45.9</v>
-      </c>
-      <c r="F34" s="15">
-        <v>1</v>
-      </c>
-      <c r="G34" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="14">
-        <v>1</v>
-      </c>
-      <c r="E35" s="15">
-        <v>-172.8</v>
-      </c>
-      <c r="F35" s="15">
-        <v>1.6</v>
-      </c>
-      <c r="G35" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="14">
-        <v>1</v>
-      </c>
-      <c r="E36" s="15">
-        <v>-36.799999999999997</v>
-      </c>
-      <c r="F36" s="15">
-        <v>1.3</v>
-      </c>
-      <c r="G36" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="14">
-        <v>1</v>
-      </c>
-      <c r="E37" s="15">
-        <v>-177.8</v>
-      </c>
-      <c r="F37" s="15">
-        <v>1.3</v>
-      </c>
-      <c r="G37" s="15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="14">
-        <v>1</v>
-      </c>
-      <c r="E38" s="15">
-        <v>-213.6</v>
-      </c>
-      <c r="F38" s="15">
-        <v>2.4</v>
-      </c>
-      <c r="G38" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="D39" s="14">
-        <v>1</v>
-      </c>
-      <c r="E39" s="15">
-        <v>-81.900000000000006</v>
-      </c>
-      <c r="F39" s="15">
-        <v>1.2</v>
-      </c>
-      <c r="G39" s="15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="14">
-        <v>1</v>
-      </c>
-      <c r="E40" s="15">
-        <v>-254.1</v>
-      </c>
-      <c r="F40" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="G40" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="14">
-        <v>1</v>
-      </c>
-      <c r="E41" s="15">
-        <v>-36.799999999999997</v>
-      </c>
-      <c r="F41" s="15">
-        <v>1.3</v>
-      </c>
-      <c r="G41" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="14">
-        <v>1</v>
-      </c>
-      <c r="E42" s="15">
-        <v>-177.8</v>
-      </c>
-      <c r="F42" s="15">
-        <v>1.3</v>
-      </c>
-      <c r="G42" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="14">
-        <v>1</v>
-      </c>
-      <c r="E43" s="15">
-        <v>-166.7</v>
-      </c>
-      <c r="F43" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="G43" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="14">
-        <v>1</v>
-      </c>
-      <c r="E45" s="15">
-        <v>-4.9000000000000004</v>
-      </c>
-      <c r="F45" s="15">
-        <v>1</v>
-      </c>
-      <c r="G45" s="15">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" s="14">
-        <v>1</v>
-      </c>
-      <c r="E46" s="15">
-        <v>-189.4</v>
-      </c>
-      <c r="F46" s="15">
-        <v>2</v>
-      </c>
-      <c r="G46" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" s="14">
-        <v>1</v>
-      </c>
-      <c r="E47" s="15">
-        <v>-117.8</v>
-      </c>
-      <c r="F47" s="15">
-        <v>2.1</v>
-      </c>
-      <c r="G47" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="14">
-        <v>1</v>
-      </c>
-      <c r="E48" s="15">
-        <v>-56.3</v>
-      </c>
-      <c r="F48" s="15">
-        <v>1</v>
-      </c>
-      <c r="G48" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49" s="14">
-        <v>1</v>
-      </c>
-      <c r="E49" s="15">
-        <v>-177.8</v>
-      </c>
-      <c r="F49" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="G49" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" s="14">
-        <v>1</v>
-      </c>
-      <c r="E50" s="15">
-        <v>-67.2</v>
-      </c>
-      <c r="F50" s="15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G50" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51" s="14">
-        <v>1</v>
-      </c>
-      <c r="E51" s="15">
-        <v>-254.1</v>
-      </c>
-      <c r="F51" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="G51" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="14">
-        <v>1</v>
-      </c>
-      <c r="E52" s="15">
-        <v>-206.2</v>
-      </c>
-      <c r="F52" s="15">
-        <v>1.7</v>
-      </c>
-      <c r="G52" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="14">
-        <v>1</v>
-      </c>
-      <c r="E53" s="15">
-        <v>-179.3</v>
-      </c>
-      <c r="F53" s="15">
-        <v>1.7</v>
-      </c>
-      <c r="G53" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="14">
-        <v>1</v>
-      </c>
-      <c r="E54" s="15">
-        <v>-172.8</v>
-      </c>
-      <c r="F54" s="15">
-        <v>1.6</v>
-      </c>
-      <c r="G54" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="14">
-        <v>1</v>
-      </c>
-      <c r="E55" s="15">
-        <v>-271.89999999999998</v>
-      </c>
-      <c r="F55" s="15">
-        <v>2</v>
-      </c>
-      <c r="G55" s="15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="14">
-        <v>1</v>
-      </c>
-      <c r="E56" s="15">
-        <v>-81.3</v>
-      </c>
-      <c r="F56" s="15">
-        <v>1.8</v>
-      </c>
-      <c r="G56" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57" s="14">
-        <v>1</v>
-      </c>
-      <c r="E57" s="15">
-        <v>-263</v>
-      </c>
-      <c r="F57" s="15">
-        <v>2.5</v>
-      </c>
-      <c r="G57" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D58" s="14">
-        <v>1</v>
-      </c>
-      <c r="E58" s="15">
-        <v>-179.3</v>
-      </c>
-      <c r="F58" s="15">
-        <v>1.9</v>
-      </c>
-      <c r="G58" s="15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" s="14">
-        <v>1</v>
-      </c>
-      <c r="E59" s="41">
-        <v>-67.2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" s="14">
-        <v>1</v>
-      </c>
-      <c r="E60" s="41">
-        <v>-263.60000000000002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="14">
-        <v>1</v>
-      </c>
-      <c r="E61" s="41">
-        <v>-172.8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="14">
-        <v>1</v>
-      </c>
-      <c r="E62" s="41">
-        <v>-85.4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" s="14">
-        <v>1</v>
-      </c>
-      <c r="E63" s="41">
-        <v>-271.89999999999998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="C71" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="14">
-        <v>1</v>
-      </c>
-    </row>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" ht="16.2" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="H1:H3"/>
@@ -7740,175 +6822,175 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>117</v>
+        <v>60</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>76</v>
+      <c r="B2" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>66</v>
+        <v>81</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>65</v>
+        <v>82</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>78</v>
+        <v>65</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>74</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+        <v>83</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>79</v>
+        <v>66</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
+        <v>208</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>76</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
+        <v>84</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+        <v>136</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+        <v>207</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>83</v>
+        <v>70</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+        <v>209</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+        <v>85</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>84</v>
+      <c r="B12" s="19" t="s">
+        <v>80</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+        <v>210</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7935,24 +7017,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>117</v>
+        <v>211</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B2" s="15">
         <v>768.2</v>
@@ -7960,16 +7042,16 @@
       <c r="C2" s="15">
         <v>10</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>233</v>
+      <c r="D2" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B3" s="15">
         <v>895.7</v>
@@ -7977,16 +7059,16 @@
       <c r="C3" s="15">
         <v>10</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>234</v>
+      <c r="D3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B4" s="15">
         <v>1217.5</v>
@@ -7995,15 +7077,15 @@
         <v>10</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B5" s="15">
         <v>1042.8</v>
@@ -8014,7 +7096,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B6" s="15">
         <v>1357.2</v>
@@ -8025,7 +7107,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B7" s="15">
         <v>1373.3</v>
@@ -8036,7 +7118,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B8" s="15">
         <v>1196.8</v>
@@ -8047,7 +7129,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B9" s="15">
         <v>1522.3</v>
@@ -8058,7 +7140,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B10" s="15">
         <v>1350.6</v>
@@ -8069,7 +7151,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B11" s="15">
         <v>1665.6</v>
@@ -8080,7 +7162,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B12" s="15">
         <v>1816.6</v>
@@ -8091,7 +7173,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B13" s="15">
         <v>2000.3</v>
@@ -8102,7 +7184,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B14" s="15">
         <v>1786.4</v>
@@ -8113,7 +7195,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B15" s="15">
         <v>2243.6</v>
@@ -8124,7 +7206,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B16" s="15">
         <v>2575.6</v>
@@ -8135,7 +7217,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B17" s="15">
         <v>3034.2</v>
@@ -8146,7 +7228,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B18" s="15">
         <v>40.1</v>
@@ -8157,7 +7239,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B19" s="15">
         <v>89.9</v>
@@ -8168,7 +7250,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B20" s="15">
         <v>139.6</v>
@@ -8211,27 +7293,27 @@
         <v>11</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>4</v>
@@ -8242,22 +7324,22 @@
       <c r="D2" s="15">
         <v>3</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="19">
         <v>-192</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="19">
         <v>3.4</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>4</v>
@@ -8272,7 +7354,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8289,15 +7371,15 @@
         <v>3</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>4</v>
@@ -8309,15 +7391,15 @@
         <v>3</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>4</v>
@@ -8329,10 +7411,10 @@
         <v>3</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -8349,10 +7431,10 @@
         <v>3</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -8413,7 +7495,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>4</v>
@@ -8427,7 +7509,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>4</v>
@@ -8450,275 +7532,275 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.88671875" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="90.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="28"/>
+    <col min="1" max="1" width="23.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.88671875" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="90.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C7" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="B11" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>239</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="C2" s="29" t="s">
+      <c r="C11" s="28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>284</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
-        <v>286</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
-        <v>287</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
-        <v>288</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
-        <v>289</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30" t="s">
-        <v>266</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>269</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>224</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
-        <v>245</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>247</v>
+      <c r="B22" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug with step-wise scale normalization.
</commit_message>
<xml_diff>
--- a/GCIRMS_Processor/GCIRMS Template.xlsx
+++ b/GCIRMS_Processor/GCIRMS Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D8F2D9-3EDB-4628-9CEB-AB76E01FF4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DF7505-92DE-4D06-87C8-EBC1DF1E3030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -706,18 +706,6 @@
     <t>initial_value</t>
   </si>
   <si>
-    <t>size_toosmall_peak_action</t>
-  </si>
-  <si>
-    <t>size_small_peak_action</t>
-  </si>
-  <si>
-    <t>size_normal_peak_action</t>
-  </si>
-  <si>
-    <t>size_large_peak_action</t>
-  </si>
-  <si>
     <t>acceptable_peak_units</t>
   </si>
   <si>
@@ -1276,6 +1264,18 @@
   </si>
   <si>
     <t>Decide to indclude (or exclude) size standards when calculating control performance.</t>
+  </si>
+  <si>
+    <t>size_toosmall_peak_option</t>
+  </si>
+  <si>
+    <t>size_small_peak_option</t>
+  </si>
+  <si>
+    <t>size_normal_peak_option</t>
+  </si>
+  <si>
+    <t>size_large_peak_option</t>
   </si>
 </sst>
 </file>
@@ -1745,6 +1745,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1761,24 +1779,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2150,7 +2150,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2188,35 +2188,35 @@
     </row>
     <row r="6" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>153</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2354,10 +2354,10 @@
         <v>19</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>51</v>
@@ -2378,7 +2378,7 @@
         <v>54</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="U2" s="5" t="str">
         <f>INDEX(U7:U8,MATCH(T10,T7:T8,0))</f>
@@ -2418,10 +2418,10 @@
         <v>19</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>51</v>
@@ -2442,10 +2442,10 @@
         <v>52</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="V3" s="5">
         <v>46.7</v>
@@ -2481,10 +2481,10 @@
         <v>19</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>53</v>
@@ -2502,13 +2502,13 @@
         <v>46.7</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="V4" s="5">
         <f>V2-43.93</f>
@@ -2545,10 +2545,10 @@
         <v>19</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>53</v>
@@ -2596,7 +2596,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K6" s="4" t="str">
         <f>Samples!$A$2</f>
@@ -2621,10 +2621,10 @@
         <v>106</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -2657,7 +2657,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K7" s="4" t="str">
         <f>Samples!$A$2</f>
@@ -2683,10 +2683,10 @@
         <v>48.04999999999999</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2719,7 +2719,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K8" s="4" t="str">
         <f>Samples!$A$3</f>
@@ -2742,10 +2742,10 @@
       </c>
       <c r="S8" s="6"/>
       <c r="T8" s="33" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -2778,7 +2778,7 @@
         <v>2</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K9" s="4" t="str">
         <f>Samples!$A$3</f>
@@ -2801,7 +2801,7 @@
       </c>
       <c r="S9" s="8"/>
       <c r="T9" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="U9" s="10"/>
     </row>
@@ -2835,7 +2835,7 @@
         <v>3</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K10" s="4" t="str">
         <f>Samples!$A$4</f>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="S10" s="8"/>
       <c r="T10" s="34" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="U10" s="10"/>
     </row>
@@ -2892,7 +2892,7 @@
         <v>3</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K11" s="4" t="str">
         <f>Samples!$A$4</f>
@@ -2945,7 +2945,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K12" s="4" t="str">
         <f>Samples!$A$5</f>
@@ -3002,7 +3002,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K13" s="4" t="str">
         <f>Samples!$A$5</f>
@@ -3068,10 +3068,10 @@
         <v>19</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>53</v>
@@ -3127,10 +3127,10 @@
         <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>53</v>
@@ -3186,10 +3186,10 @@
         <v>37</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>40</v>
@@ -3211,14 +3211,14 @@
         <v>107</v>
       </c>
       <c r="U16" s="9"/>
-      <c r="V16" s="46" t="s">
+      <c r="V16" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="W16" s="47"/>
-      <c r="X16" s="52" t="s">
+      <c r="W16" s="53"/>
+      <c r="X16" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="Y16" s="53"/>
+      <c r="Y16" s="47"/>
       <c r="Z16" s="10"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -3251,10 +3251,10 @@
         <v>38</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>40</v>
@@ -3274,10 +3274,10 @@
       <c r="S17" s="8"/>
       <c r="T17" s="59"/>
       <c r="U17" s="9"/>
-      <c r="V17" s="48"/>
-      <c r="W17" s="49"/>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="55"/>
+      <c r="V17" s="54"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
       <c r="Z17" s="10"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -3310,10 +3310,10 @@
         <v>39</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>40</v>
@@ -3333,10 +3333,10 @@
       <c r="S18" s="8"/>
       <c r="T18" s="60"/>
       <c r="U18" s="9"/>
-      <c r="V18" s="50"/>
-      <c r="W18" s="51"/>
-      <c r="X18" s="56"/>
-      <c r="Y18" s="57"/>
+      <c r="V18" s="56"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="51"/>
       <c r="Z18" s="10"/>
     </row>
     <row r="19" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3369,10 +3369,10 @@
         <v>40</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>40</v>
@@ -3394,14 +3394,14 @@
         <v>108</v>
       </c>
       <c r="U19" s="9"/>
-      <c r="V19" s="46" t="s">
+      <c r="V19" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="W19" s="47"/>
-      <c r="X19" s="52" t="s">
+      <c r="W19" s="53"/>
+      <c r="X19" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="Y19" s="53"/>
+      <c r="Y19" s="47"/>
       <c r="Z19" s="10"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -3434,10 +3434,10 @@
         <v>41</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>40</v>
@@ -3457,10 +3457,10 @@
       <c r="S20" s="8"/>
       <c r="T20" s="59"/>
       <c r="U20" s="9"/>
-      <c r="V20" s="48"/>
-      <c r="W20" s="49"/>
-      <c r="X20" s="54"/>
-      <c r="Y20" s="55"/>
+      <c r="V20" s="54"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="49"/>
       <c r="Z20" s="10"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -3493,10 +3493,10 @@
         <v>42</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>40</v>
@@ -3516,10 +3516,10 @@
       <c r="S21" s="8"/>
       <c r="T21" s="60"/>
       <c r="U21" s="9"/>
-      <c r="V21" s="50"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="56"/>
-      <c r="Y21" s="57"/>
+      <c r="V21" s="56"/>
+      <c r="W21" s="57"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="51"/>
       <c r="Z21" s="10"/>
     </row>
     <row r="22" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3552,7 +3552,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>9</v>
@@ -3576,14 +3576,14 @@
         <v>116</v>
       </c>
       <c r="U22" s="8"/>
-      <c r="V22" s="46" t="s">
+      <c r="V22" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="W22" s="47"/>
-      <c r="X22" s="52" t="s">
+      <c r="W22" s="53"/>
+      <c r="X22" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="Y22" s="53"/>
+      <c r="Y22" s="47"/>
       <c r="Z22" s="10"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -3616,7 +3616,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>9</v>
@@ -3638,10 +3638,10 @@
       </c>
       <c r="T23" s="59"/>
       <c r="U23" s="8"/>
-      <c r="V23" s="48"/>
-      <c r="W23" s="49"/>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="55"/>
+      <c r="V23" s="54"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="48"/>
+      <c r="Y23" s="49"/>
       <c r="Z23" s="10"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -3674,10 +3674,10 @@
         <v>19</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>53</v>
@@ -3696,10 +3696,10 @@
       </c>
       <c r="T24" s="60"/>
       <c r="U24" s="8"/>
-      <c r="V24" s="50"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="56"/>
-      <c r="Y24" s="57"/>
+      <c r="V24" s="56"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="51"/>
       <c r="Z24" s="10"/>
     </row>
     <row r="25" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3732,10 +3732,10 @@
         <v>19</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>53</v>
@@ -3756,14 +3756,14 @@
         <v>110</v>
       </c>
       <c r="U25" s="8"/>
-      <c r="V25" s="46" t="s">
+      <c r="V25" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="W25" s="47"/>
-      <c r="X25" s="52" t="s">
+      <c r="W25" s="53"/>
+      <c r="X25" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="Y25" s="53"/>
+      <c r="Y25" s="47"/>
       <c r="Z25" s="10"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3796,7 +3796,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K26" s="4" t="str">
         <f>Samples!$A$6</f>
@@ -3819,10 +3819,10 @@
       </c>
       <c r="T26" s="62"/>
       <c r="U26" s="8"/>
-      <c r="V26" s="48"/>
-      <c r="W26" s="49"/>
-      <c r="X26" s="54"/>
-      <c r="Y26" s="55"/>
+      <c r="V26" s="54"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="48"/>
+      <c r="Y26" s="49"/>
       <c r="Z26" s="10"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -3855,7 +3855,7 @@
         <v>5</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K27" s="4" t="str">
         <f>Samples!$A$6</f>
@@ -3878,10 +3878,10 @@
       </c>
       <c r="T27" s="62"/>
       <c r="U27" s="8"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="51"/>
-      <c r="X27" s="56"/>
-      <c r="Y27" s="57"/>
+      <c r="V27" s="56"/>
+      <c r="W27" s="57"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="51"/>
       <c r="Z27" s="10"/>
     </row>
     <row r="28" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3914,7 +3914,7 @@
         <v>6</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K28" s="4" t="str">
         <f>Samples!$A$7</f>
@@ -3937,14 +3937,14 @@
       </c>
       <c r="T28" s="62"/>
       <c r="U28" s="8"/>
-      <c r="V28" s="46" t="s">
+      <c r="V28" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="W28" s="47"/>
-      <c r="X28" s="52" t="s">
+      <c r="W28" s="53"/>
+      <c r="X28" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="Y28" s="53"/>
+      <c r="Y28" s="47"/>
       <c r="Z28" s="10"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -3977,7 +3977,7 @@
         <v>6</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K29" s="4" t="str">
         <f>Samples!$A$7</f>
@@ -4000,10 +4000,10 @@
       </c>
       <c r="T29" s="62"/>
       <c r="U29" s="8"/>
-      <c r="V29" s="48"/>
-      <c r="W29" s="49"/>
-      <c r="X29" s="54"/>
-      <c r="Y29" s="55"/>
+      <c r="V29" s="54"/>
+      <c r="W29" s="55"/>
+      <c r="X29" s="48"/>
+      <c r="Y29" s="49"/>
       <c r="Z29" s="10"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -4036,7 +4036,7 @@
         <v>7</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K30" s="4" t="str">
         <f>Samples!$A$8</f>
@@ -4059,10 +4059,10 @@
       </c>
       <c r="T30" s="63"/>
       <c r="U30" s="8"/>
-      <c r="V30" s="50"/>
-      <c r="W30" s="51"/>
-      <c r="X30" s="56"/>
-      <c r="Y30" s="57"/>
+      <c r="V30" s="56"/>
+      <c r="W30" s="57"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="51"/>
       <c r="Z30" s="10"/>
     </row>
     <row r="31" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4095,7 +4095,7 @@
         <v>7</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K31" s="4" t="str">
         <f>Samples!$A$8</f>
@@ -4116,14 +4116,14 @@
         <f t="shared" si="5"/>
         <v>61.75</v>
       </c>
-      <c r="V31" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="W31" s="47"/>
-      <c r="X31" s="52" t="s">
-        <v>203</v>
-      </c>
-      <c r="Y31" s="53"/>
+      <c r="V31" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="W31" s="53"/>
+      <c r="X31" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y31" s="47"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
@@ -4155,7 +4155,7 @@
         <v>8</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K32" s="4" t="str">
         <f>Samples!$A$9</f>
@@ -4176,10 +4176,10 @@
         <f t="shared" si="5"/>
         <v>61.75</v>
       </c>
-      <c r="V32" s="48"/>
-      <c r="W32" s="49"/>
-      <c r="X32" s="54"/>
-      <c r="Y32" s="55"/>
+      <c r="V32" s="54"/>
+      <c r="W32" s="55"/>
+      <c r="X32" s="48"/>
+      <c r="Y32" s="49"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
@@ -4211,7 +4211,7 @@
         <v>8</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K33" s="4" t="str">
         <f>Samples!$A$9</f>
@@ -4232,10 +4232,10 @@
         <f t="shared" si="5"/>
         <v>61.75</v>
       </c>
-      <c r="V33" s="50"/>
-      <c r="W33" s="51"/>
-      <c r="X33" s="56"/>
-      <c r="Y33" s="57"/>
+      <c r="V33" s="56"/>
+      <c r="W33" s="57"/>
+      <c r="X33" s="50"/>
+      <c r="Y33" s="51"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
@@ -4267,10 +4267,10 @@
         <v>19</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>53</v>
@@ -4287,14 +4287,14 @@
         <f t="shared" si="5"/>
         <v>46.7</v>
       </c>
-      <c r="V34" s="46" t="s">
+      <c r="V34" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="W34" s="47"/>
-      <c r="X34" s="52" t="s">
+      <c r="W34" s="53"/>
+      <c r="X34" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="Y34" s="53"/>
+      <c r="Y34" s="47"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
@@ -4326,10 +4326,10 @@
         <v>19</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>53</v>
@@ -4346,10 +4346,10 @@
         <f t="shared" si="5"/>
         <v>46.7</v>
       </c>
-      <c r="V35" s="48"/>
-      <c r="W35" s="49"/>
-      <c r="X35" s="54"/>
-      <c r="Y35" s="55"/>
+      <c r="V35" s="54"/>
+      <c r="W35" s="55"/>
+      <c r="X35" s="48"/>
+      <c r="Y35" s="49"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
@@ -4381,10 +4381,10 @@
         <v>21</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>41</v>
@@ -4401,10 +4401,10 @@
         <f t="shared" ref="Q36:Q55" si="8">INDEX(V$2:V$4,MATCH(O36,U$2:U$4,0))</f>
         <v>46.7</v>
       </c>
-      <c r="V36" s="50"/>
-      <c r="W36" s="51"/>
-      <c r="X36" s="56"/>
-      <c r="Y36" s="57"/>
+      <c r="V36" s="56"/>
+      <c r="W36" s="57"/>
+      <c r="X36" s="50"/>
+      <c r="Y36" s="51"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
@@ -4436,10 +4436,10 @@
         <v>21</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>41</v>
@@ -4487,10 +4487,10 @@
         <v>37</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L38" s="4" t="s">
         <v>40</v>
@@ -4538,10 +4538,10 @@
         <v>38</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>40</v>
@@ -4589,10 +4589,10 @@
         <v>39</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L40" s="4" t="s">
         <v>40</v>
@@ -4640,10 +4640,10 @@
         <v>40</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>40</v>
@@ -4691,10 +4691,10 @@
         <v>41</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>40</v>
@@ -4742,10 +4742,10 @@
         <v>42</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L43" s="4" t="s">
         <v>40</v>
@@ -4793,10 +4793,10 @@
         <v>19</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>53</v>
@@ -4844,10 +4844,10 @@
         <v>19</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>53</v>
@@ -4895,7 +4895,7 @@
         <v>9</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K46" s="4" t="str">
         <f>Samples!$A$10</f>
@@ -4947,7 +4947,7 @@
         <v>9</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K47" s="4" t="str">
         <f>Samples!$A$10</f>
@@ -4999,7 +4999,7 @@
         <v>10</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K48" s="4" t="str">
         <f>Samples!$A$11</f>
@@ -5051,7 +5051,7 @@
         <v>10</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K49" s="4" t="str">
         <f>Samples!$A$11</f>
@@ -5103,7 +5103,7 @@
         <v>11</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K50" s="4" t="str">
         <f>Samples!$A$12</f>
@@ -5155,7 +5155,7 @@
         <v>11</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K51" s="4" t="str">
         <f>Samples!$A$12</f>
@@ -5207,7 +5207,7 @@
         <v>12</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K52" s="4" t="str">
         <f>Samples!$A$13</f>
@@ -5259,7 +5259,7 @@
         <v>12</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K53" s="4" t="str">
         <f>Samples!$A$13</f>
@@ -5311,10 +5311,10 @@
         <v>19</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>53</v>
@@ -5362,10 +5362,10 @@
         <v>19</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>53</v>
@@ -5406,20 +5406,20 @@
         <v>24</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I56" s="4">
         <v>54</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
@@ -5860,11 +5860,6 @@
     <sortCondition descending="1" ref="A41:A46"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="X22:Y24"/>
-    <mergeCell ref="V25:W27"/>
-    <mergeCell ref="X25:Y27"/>
-    <mergeCell ref="V28:W30"/>
-    <mergeCell ref="X28:Y30"/>
     <mergeCell ref="V34:W36"/>
     <mergeCell ref="X34:Y36"/>
     <mergeCell ref="T13:T15"/>
@@ -5881,6 +5876,11 @@
     <mergeCell ref="V31:W33"/>
     <mergeCell ref="X31:Y33"/>
     <mergeCell ref="V22:W24"/>
+    <mergeCell ref="X22:Y24"/>
+    <mergeCell ref="V25:W27"/>
+    <mergeCell ref="X25:Y27"/>
+    <mergeCell ref="V28:W30"/>
+    <mergeCell ref="X28:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
@@ -5939,7 +5939,7 @@
         <v>57</v>
       </c>
       <c r="H1" s="58" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>124</v>
@@ -5950,13 +5950,13 @@
     </row>
     <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E2" s="13">
         <v>20</v>
@@ -5968,18 +5968,18 @@
         <v>35</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E3" s="13">
         <v>20</v>
@@ -5991,18 +5991,18 @@
         <v>22</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="45" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E4" s="13">
         <v>20</v>
@@ -6019,13 +6019,13 @@
     </row>
     <row r="5" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E5" s="13">
         <v>20</v>
@@ -6042,13 +6042,13 @@
     </row>
     <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E6" s="13">
         <v>20</v>
@@ -6060,18 +6060,18 @@
         <v>3</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E7" s="13">
         <v>20</v>
@@ -6088,13 +6088,13 @@
     </row>
     <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="45" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E8" s="13">
         <v>20</v>
@@ -6111,13 +6111,13 @@
     </row>
     <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E9" s="13">
         <v>20</v>
@@ -6128,13 +6128,13 @@
     </row>
     <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="45" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E10" s="13">
         <v>20</v>
@@ -6145,13 +6145,13 @@
     </row>
     <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E11" s="13">
         <v>20</v>
@@ -6162,13 +6162,13 @@
     </row>
     <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="45" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E12" s="13">
         <v>20</v>
@@ -6178,13 +6178,13 @@
     </row>
     <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E13" s="13">
         <v>20</v>
@@ -6347,7 +6347,7 @@
     <col min="11" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>35</v>
       </c>
@@ -6379,7 +6379,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>49</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>49</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -6471,7 +6471,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>49</v>
       </c>
@@ -6498,10 +6498,10 @@
         <v>109</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
@@ -6528,10 +6528,10 @@
         <v>8</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>9</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>9</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>9</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>10</v>
       </c>
@@ -6652,7 +6652,7 @@
         <v>-204.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>10</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>-146.6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>10</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>-161.1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>10</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>-197.9</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>10</v>
       </c>
@@ -6720,15 +6720,15 @@
         <v>-154.5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D16" s="13">
         <v>1</v>
@@ -6745,7 +6745,7 @@
     </row>
     <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>17</v>
@@ -6762,7 +6762,7 @@
     </row>
     <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>18</v>
@@ -6779,7 +6779,7 @@
     </row>
     <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>46</v>
@@ -6796,7 +6796,7 @@
     </row>
     <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>47</v>
@@ -6813,7 +6813,7 @@
     </row>
     <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>50</v>
@@ -6828,9 +6828,9 @@
         <v>-271.89999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>16</v>
@@ -6851,9 +6851,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>17</v>
@@ -6874,9 +6874,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>18</v>
@@ -6897,9 +6897,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>46</v>
@@ -6920,9 +6920,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>47</v>
@@ -6943,9 +6943,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>50</v>
@@ -6966,12 +6966,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>12</v>
@@ -6989,12 +6989,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>12</v>
@@ -7012,9 +7012,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>17</v>
@@ -7029,9 +7029,9 @@
         <v>-67.2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>18</v>
@@ -7046,9 +7046,9 @@
         <v>-263.60000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>46</v>
@@ -7063,9 +7063,9 @@
         <v>-172.8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>47</v>
@@ -7080,9 +7080,9 @@
         <v>-85.4</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>50</v>
@@ -7097,9 +7097,9 @@
         <v>-271.89999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>13</v>
@@ -7120,9 +7120,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>5</v>
@@ -7260,7 +7260,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="21"/>
@@ -7270,7 +7270,7 @@
         <v>67</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>83</v>
@@ -7299,7 +7299,7 @@
         <v>77</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
@@ -7312,7 +7312,7 @@
         <v>78</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -7338,7 +7338,7 @@
         <v>79</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -7368,13 +7368,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>70</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>124</v>
@@ -7385,7 +7385,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B2" s="14">
         <v>768.2</v>
@@ -7394,15 +7394,15 @@
         <v>10</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B3" s="14">
         <v>895.7</v>
@@ -7414,12 +7414,12 @@
         <v>70</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B4" s="14">
         <v>1217.5</v>
@@ -7428,15 +7428,15 @@
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B5" s="14">
         <v>1042.8</v>
@@ -7447,7 +7447,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B6" s="14">
         <v>1357.2</v>
@@ -7458,7 +7458,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B7" s="14">
         <v>1373.3</v>
@@ -7469,7 +7469,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B8" s="14">
         <v>1196.8</v>
@@ -7480,7 +7480,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B9" s="14">
         <v>1522.3</v>
@@ -7491,7 +7491,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B10" s="14">
         <v>1350.6</v>
@@ -7502,7 +7502,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B11" s="14">
         <v>1665.6</v>
@@ -7513,7 +7513,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B12" s="14">
         <v>1816.6</v>
@@ -7524,7 +7524,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B13" s="14">
         <v>2000.3</v>
@@ -7535,7 +7535,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B14" s="14">
         <v>1786.4</v>
@@ -7546,7 +7546,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B15" s="14">
         <v>2243.6</v>
@@ -7557,7 +7557,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B16" s="14">
         <v>2575.6</v>
@@ -7568,7 +7568,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B17" s="14">
         <v>3034.2</v>
@@ -7579,7 +7579,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B18" s="14">
         <v>40.1</v>
@@ -7590,7 +7590,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B19" s="14">
         <v>89.9</v>
@@ -7601,7 +7601,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B20" s="14">
         <v>139.6</v>
@@ -7644,16 +7644,16 @@
         <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>124</v>
@@ -7722,10 +7722,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7742,10 +7742,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7762,7 +7762,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>137</v>
@@ -7782,7 +7782,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H7" s="15" t="s">
         <v>138</v>
@@ -7874,10 +7874,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C14" s="14">
         <v>4</v>
@@ -7897,7 +7897,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7929,19 +7929,19 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>85</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7952,13 +7952,13 @@
         <v>86</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>154</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7969,13 +7969,13 @@
         <v>87</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>60</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7986,18 +7986,18 @@
         <v>88</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>100</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -8008,7 +8008,7 @@
         <v>89</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -8019,18 +8019,18 @@
         <v>90</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -8038,89 +8038,89 @@
         <v>97</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
-        <v>155</v>
+        <v>284</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>156</v>
+        <v>285</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
-        <v>157</v>
+        <v>286</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
-        <v>158</v>
+        <v>287</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>90</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -8131,18 +8131,18 @@
         <v>91</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -8150,10 +8150,10 @@
         <v>99</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -8161,21 +8161,21 @@
         <v>99</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added drop-down menus for the `Initials` tab.
</commit_message>
<xml_diff>
--- a/GCIRMS_Processor/GCIRMS Template.xlsx
+++ b/GCIRMS_Processor/GCIRMS Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DF7505-92DE-4D06-87C8-EBC1DF1E3030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944D861D-FEFC-43B8-B79E-EC1397BA5A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Standards!$A$1:$G$15</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="303">
   <si>
     <t>id1</t>
   </si>
@@ -1131,12 +1131,6 @@
     <t>derivatization_option</t>
   </si>
   <si>
-    <t>Template-defined derivative \u03B4D.</t>
-  </si>
-  <si>
-    <t>Choose where to source the δD of the derivative hydrogen.</t>
-  </si>
-  <si>
     <t>Sample Type</t>
   </si>
   <si>
@@ -1257,6 +1251,51 @@
     <t>VA-29</t>
   </si>
   <si>
+    <t>size_toosmall_peak_option</t>
+  </si>
+  <si>
+    <t>size_small_peak_option</t>
+  </si>
+  <si>
+    <t>size_normal_peak_option</t>
+  </si>
+  <si>
+    <t>size_large_peak_option</t>
+  </si>
+  <si>
+    <t>option_1</t>
+  </si>
+  <si>
+    <t>option_2</t>
+  </si>
+  <si>
+    <t>option_3</t>
+  </si>
+  <si>
+    <t>Assigned by retention time matching with Retention Times sheet.</t>
+  </si>
+  <si>
+    <t>Linear interpolation between adjacent drift samples (use this when drift appears non-linear)</t>
+  </si>
+  <si>
+    <t>Linear regression across all drift samples (use this when drift appears linear)</t>
+  </si>
+  <si>
+    <t>No size effect correction.</t>
+  </si>
+  <si>
+    <t>Peak Area (Vs)</t>
+  </si>
+  <si>
+    <t>Linear model</t>
+  </si>
+  <si>
+    <t>Log-Transformed linear model</t>
+  </si>
+  <si>
+    <t>Use 'Small' size effect function.</t>
+  </si>
+  <si>
     <t>size_for_control</t>
   </si>
   <si>
@@ -1266,16 +1305,22 @@
     <t>Decide to indclude (or exclude) size standards when calculating control performance.</t>
   </si>
   <si>
-    <t>size_toosmall_peak_option</t>
-  </si>
-  <si>
-    <t>size_small_peak_option</t>
-  </si>
-  <si>
-    <t>size_normal_peak_option</t>
-  </si>
-  <si>
-    <t>size_large_peak_option</t>
+    <t>Exclude</t>
+  </si>
+  <si>
+    <t>Linear regression across all normalization standards (use this if you drift-correct)</t>
+  </si>
+  <si>
+    <t>Choose where to source the δ2H of the derivative hydrogen.</t>
+  </si>
+  <si>
+    <t>Template-defined derivative \u03B4\u00b2H.</t>
+  </si>
+  <si>
+    <t>Derivatization standard in sequence \u03B4\u00b2H.</t>
+  </si>
+  <si>
+    <t>Do not correct for derivative hydrogen.</t>
   </si>
 </sst>
 </file>
@@ -1615,7 +1660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1836,6 +1881,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2354,10 +2408,10 @@
         <v>19</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>51</v>
@@ -2378,7 +2432,7 @@
         <v>54</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="U2" s="5" t="str">
         <f>INDEX(U7:U8,MATCH(T10,T7:T8,0))</f>
@@ -2418,10 +2472,10 @@
         <v>19</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>51</v>
@@ -2442,10 +2496,10 @@
         <v>52</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="V3" s="5">
         <v>46.7</v>
@@ -2481,10 +2535,10 @@
         <v>19</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>53</v>
@@ -2505,10 +2559,10 @@
         <v>198</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="V4" s="5">
         <f>V2-43.93</f>
@@ -2545,10 +2599,10 @@
         <v>19</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>53</v>
@@ -2596,7 +2650,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K6" s="4" t="str">
         <f>Samples!$A$2</f>
@@ -2621,10 +2675,10 @@
         <v>106</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -2657,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K7" s="4" t="str">
         <f>Samples!$A$2</f>
@@ -2683,10 +2737,10 @@
         <v>48.04999999999999</v>
       </c>
       <c r="T7" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="U7" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2719,7 +2773,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K8" s="4" t="str">
         <f>Samples!$A$3</f>
@@ -2742,10 +2796,10 @@
       </c>
       <c r="S8" s="6"/>
       <c r="T8" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="U8" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -2778,7 +2832,7 @@
         <v>2</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K9" s="4" t="str">
         <f>Samples!$A$3</f>
@@ -2801,7 +2855,7 @@
       </c>
       <c r="S9" s="8"/>
       <c r="T9" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="U9" s="10"/>
     </row>
@@ -2835,7 +2889,7 @@
         <v>3</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K10" s="4" t="str">
         <f>Samples!$A$4</f>
@@ -2858,7 +2912,7 @@
       </c>
       <c r="S10" s="8"/>
       <c r="T10" s="34" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="U10" s="10"/>
     </row>
@@ -2892,7 +2946,7 @@
         <v>3</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K11" s="4" t="str">
         <f>Samples!$A$4</f>
@@ -2945,7 +2999,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K12" s="4" t="str">
         <f>Samples!$A$5</f>
@@ -3002,7 +3056,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K13" s="4" t="str">
         <f>Samples!$A$5</f>
@@ -3068,10 +3122,10 @@
         <v>19</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>53</v>
@@ -3127,10 +3181,10 @@
         <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>53</v>
@@ -3186,10 +3240,10 @@
         <v>37</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>40</v>
@@ -3251,10 +3305,10 @@
         <v>38</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>40</v>
@@ -3310,10 +3364,10 @@
         <v>39</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>40</v>
@@ -3369,10 +3423,10 @@
         <v>40</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>40</v>
@@ -3434,10 +3488,10 @@
         <v>41</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>40</v>
@@ -3493,10 +3547,10 @@
         <v>42</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>40</v>
@@ -3552,7 +3606,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>9</v>
@@ -3616,7 +3670,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>9</v>
@@ -3674,10 +3728,10 @@
         <v>19</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>53</v>
@@ -3732,10 +3786,10 @@
         <v>19</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>53</v>
@@ -3796,7 +3850,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K26" s="4" t="str">
         <f>Samples!$A$6</f>
@@ -3855,7 +3909,7 @@
         <v>5</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K27" s="4" t="str">
         <f>Samples!$A$6</f>
@@ -3914,7 +3968,7 @@
         <v>6</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K28" s="4" t="str">
         <f>Samples!$A$7</f>
@@ -3977,7 +4031,7 @@
         <v>6</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K29" s="4" t="str">
         <f>Samples!$A$7</f>
@@ -4036,7 +4090,7 @@
         <v>7</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K30" s="4" t="str">
         <f>Samples!$A$8</f>
@@ -4095,7 +4149,7 @@
         <v>7</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K31" s="4" t="str">
         <f>Samples!$A$8</f>
@@ -4155,7 +4209,7 @@
         <v>8</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K32" s="4" t="str">
         <f>Samples!$A$9</f>
@@ -4211,7 +4265,7 @@
         <v>8</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K33" s="4" t="str">
         <f>Samples!$A$9</f>
@@ -4267,10 +4321,10 @@
         <v>19</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>53</v>
@@ -4326,10 +4380,10 @@
         <v>19</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>53</v>
@@ -4381,10 +4435,10 @@
         <v>21</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>41</v>
@@ -4436,10 +4490,10 @@
         <v>21</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>41</v>
@@ -4487,10 +4541,10 @@
         <v>37</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L38" s="4" t="s">
         <v>40</v>
@@ -4538,10 +4592,10 @@
         <v>38</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>40</v>
@@ -4589,10 +4643,10 @@
         <v>39</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L40" s="4" t="s">
         <v>40</v>
@@ -4640,10 +4694,10 @@
         <v>40</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>40</v>
@@ -4691,10 +4745,10 @@
         <v>41</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>40</v>
@@ -4742,10 +4796,10 @@
         <v>42</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L43" s="4" t="s">
         <v>40</v>
@@ -4793,10 +4847,10 @@
         <v>19</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>53</v>
@@ -4844,10 +4898,10 @@
         <v>19</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>53</v>
@@ -4895,7 +4949,7 @@
         <v>9</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K46" s="4" t="str">
         <f>Samples!$A$10</f>
@@ -4947,7 +5001,7 @@
         <v>9</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K47" s="4" t="str">
         <f>Samples!$A$10</f>
@@ -4999,7 +5053,7 @@
         <v>10</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K48" s="4" t="str">
         <f>Samples!$A$11</f>
@@ -5051,7 +5105,7 @@
         <v>10</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K49" s="4" t="str">
         <f>Samples!$A$11</f>
@@ -5103,7 +5157,7 @@
         <v>11</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K50" s="4" t="str">
         <f>Samples!$A$12</f>
@@ -5155,7 +5209,7 @@
         <v>11</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K51" s="4" t="str">
         <f>Samples!$A$12</f>
@@ -5207,7 +5261,7 @@
         <v>12</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K52" s="4" t="str">
         <f>Samples!$A$13</f>
@@ -5259,7 +5313,7 @@
         <v>12</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K53" s="4" t="str">
         <f>Samples!$A$13</f>
@@ -5311,10 +5365,10 @@
         <v>19</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>53</v>
@@ -5362,10 +5416,10 @@
         <v>19</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>53</v>
@@ -5406,20 +5460,20 @@
         <v>24</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I56" s="4">
         <v>54</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
@@ -5950,13 +6004,13 @@
     </row>
     <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E2" s="13">
         <v>20</v>
@@ -5973,13 +6027,13 @@
     </row>
     <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E3" s="13">
         <v>20</v>
@@ -5996,13 +6050,13 @@
     </row>
     <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="45" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E4" s="13">
         <v>20</v>
@@ -6019,13 +6073,13 @@
     </row>
     <row r="5" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E5" s="13">
         <v>20</v>
@@ -6042,13 +6096,13 @@
     </row>
     <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E6" s="13">
         <v>20</v>
@@ -6065,13 +6119,13 @@
     </row>
     <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E7" s="13">
         <v>20</v>
@@ -6088,13 +6142,13 @@
     </row>
     <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="45" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E8" s="13">
         <v>20</v>
@@ -6111,13 +6165,13 @@
     </row>
     <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E9" s="13">
         <v>20</v>
@@ -6128,13 +6182,13 @@
     </row>
     <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="45" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E10" s="13">
         <v>20</v>
@@ -6145,13 +6199,13 @@
     </row>
     <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E11" s="13">
         <v>20</v>
@@ -6162,13 +6216,13 @@
     </row>
     <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="45" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E12" s="13">
         <v>20</v>
@@ -6178,13 +6232,13 @@
     </row>
     <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E13" s="13">
         <v>20</v>
@@ -6745,7 +6799,7 @@
     </row>
     <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>17</v>
@@ -6762,7 +6816,7 @@
     </row>
     <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>18</v>
@@ -6779,7 +6833,7 @@
     </row>
     <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>46</v>
@@ -6796,7 +6850,7 @@
     </row>
     <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>47</v>
@@ -6813,7 +6867,7 @@
     </row>
     <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>50</v>
@@ -6830,7 +6884,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>16</v>
@@ -6853,7 +6907,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>17</v>
@@ -6876,7 +6930,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>18</v>
@@ -6899,7 +6953,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>46</v>
@@ -6922,7 +6976,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>47</v>
@@ -6945,7 +6999,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>50</v>
@@ -6968,10 +7022,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>12</v>
@@ -6991,10 +7045,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>12</v>
@@ -7014,7 +7068,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>17</v>
@@ -7031,7 +7085,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>18</v>
@@ -7048,7 +7102,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>46</v>
@@ -7065,7 +7119,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>47</v>
@@ -7082,7 +7136,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>50</v>
@@ -7099,7 +7153,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>13</v>
@@ -7122,7 +7176,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>5</v>
@@ -7270,7 +7324,7 @@
         <v>67</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>83</v>
@@ -7894,10 +7948,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7910,7 +7964,7 @@
     <col min="6" max="16384" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>85</v>
       </c>
@@ -7926,8 +7980,18 @@
       <c r="E1" s="30" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="77" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1" s="77" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1" s="77" t="s">
+        <v>285</v>
+      </c>
+      <c r="K1" s="77"/>
+    </row>
+    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>234</v>
       </c>
@@ -7943,8 +8007,16 @@
       <c r="E2" s="19" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="78" t="s">
+        <v>235</v>
+      </c>
+      <c r="I2" s="79" t="s">
+        <v>286</v>
+      </c>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>92</v>
       </c>
@@ -7960,8 +8032,18 @@
       <c r="E3" s="19" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="79" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" s="79"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>93</v>
       </c>
@@ -7977,8 +8059,18 @@
       <c r="E4" s="19" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="79" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="79"/>
+    </row>
+    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>94</v>
       </c>
@@ -7988,8 +8080,18 @@
       <c r="C5" s="26" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="79" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="79"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>186</v>
       </c>
@@ -7999,8 +8101,18 @@
       <c r="C6" s="26" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" s="79" t="s">
+        <v>287</v>
+      </c>
+      <c r="J6" s="79" t="s">
+        <v>288</v>
+      </c>
+      <c r="K6" s="79"/>
+    </row>
+    <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>95</v>
       </c>
@@ -8010,8 +8122,14 @@
       <c r="C7" s="26" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>96</v>
       </c>
@@ -8021,29 +8139,53 @@
       <c r="C8" s="26" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="I8" s="79" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="79" t="s">
+        <v>290</v>
+      </c>
+      <c r="K8" s="79"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="I9" s="79" t="s">
+        <v>291</v>
+      </c>
+      <c r="J9" s="79" t="s">
+        <v>259</v>
+      </c>
+      <c r="K9" s="79"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>97</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="27"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>158</v>
@@ -8051,10 +8193,20 @@
       <c r="C11" s="26" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="I11" s="79" t="s">
+        <v>289</v>
+      </c>
+      <c r="J11" s="79" t="s">
+        <v>293</v>
+      </c>
+      <c r="K11" s="79"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>159</v>
@@ -8062,10 +8214,18 @@
       <c r="C12" s="26" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I12" s="79" t="s">
+        <v>289</v>
+      </c>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+    </row>
+    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>159</v>
@@ -8073,10 +8233,18 @@
       <c r="C13" s="26" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I13" s="79" t="s">
+        <v>289</v>
+      </c>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+    </row>
+    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>160</v>
@@ -8084,8 +8252,18 @@
       <c r="C14" s="26" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="I14" s="79" t="s">
+        <v>289</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="K14" s="79"/>
+    </row>
+    <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>155</v>
       </c>
@@ -8095,35 +8273,57 @@
       <c r="C15" s="26" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" s="79" t="s">
+        <v>290</v>
+      </c>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>156</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="27"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+    </row>
+    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>157</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="27"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>98</v>
       </c>
@@ -8133,19 +8333,31 @@
       <c r="C19" s="26" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="27" t="s">
+        <v>298</v>
+      </c>
+      <c r="I19" s="79" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
+    </row>
+    <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>99</v>
       </c>
@@ -8155,8 +8367,12 @@
       <c r="C21" s="26" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="27"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
+    </row>
+    <row r="22" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>99</v>
       </c>
@@ -8166,19 +8382,38 @@
       <c r="C22" s="26" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="27"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="79"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>238</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>239</v>
+        <v>300</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>240</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="I23" s="79" t="s">
+        <v>301</v>
+      </c>
+      <c r="J23" s="79" t="s">
+        <v>302</v>
+      </c>
+      <c r="K23" s="79"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B15 B18:B19 B23 B2:B9" xr:uid="{89AE0CE1-DE70-45CC-BA80-C0608274C91E}">
+      <formula1>H2:J2</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>